<commit_message>
Found test control signals
</commit_message>
<xml_diff>
--- a/Lab_2/Report/ControlSignals.xlsx
+++ b/Lab_2/Report/ControlSignals.xlsx
@@ -4,8 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Path B" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="83">
   <si>
     <t>W_EN</t>
   </si>
@@ -179,10 +178,97 @@
     <t>M_out[15:0]</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Stage</t>
+  </si>
+  <si>
+    <t>Fetch</t>
+  </si>
+  <si>
+    <t>RegRd</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>RegWr</t>
+  </si>
+  <si>
+    <t>00FF</t>
+  </si>
+  <si>
+    <t>000000</t>
+  </si>
+  <si>
+    <t>Ø0ØØ</t>
+  </si>
+  <si>
+    <t>ØØ0Ø</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ØØØØØ</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>ØØØØØØ</t>
+  </si>
+  <si>
+    <t>ØØ01</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>ØØØ</t>
+  </si>
+  <si>
+    <t>0102</t>
+  </si>
+  <si>
+    <t>ØØ00</t>
+  </si>
+  <si>
+    <t>Mem Acc</t>
+  </si>
+  <si>
+    <t>0103</t>
+  </si>
+  <si>
+    <t>brneq R2, 010F</t>
+  </si>
+  <si>
+    <t>RegWrite</t>
+  </si>
+  <si>
+    <t>1F1F</t>
+  </si>
+  <si>
+    <t>CCCC</t>
+  </si>
+  <si>
+    <t>Ø1ØØ</t>
+  </si>
+  <si>
+    <t>1ØØØ</t>
+  </si>
+  <si>
+    <t>0104</t>
+  </si>
+  <si>
+    <t>0x010F</t>
+  </si>
+  <si>
+    <t>ØØ11</t>
+  </si>
+  <si>
+    <t>0105</t>
+  </si>
+  <si>
+    <t>0214</t>
+  </si>
+  <si>
+    <t>---------10</t>
   </si>
 </sst>
 </file>
@@ -219,7 +305,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,8 +324,14 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -494,11 +586,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -515,7 +620,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -527,21 +631,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -553,13 +645,40 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1117,10 +1236,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1182,178 +1300,178 @@
       <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="17" t="s">
+      <c r="F3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="17" t="s">
+      <c r="H3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="18" t="s">
+      <c r="L3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="19" t="s">
+      <c r="N3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="17" t="s">
+      <c r="F4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="17" t="s">
+      <c r="I4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="18" t="s">
+      <c r="L4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="19" t="s">
+      <c r="N4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="17" t="s">
+      <c r="F5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="H5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="17" t="s">
+      <c r="J5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="18" t="s">
+      <c r="L5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" s="19" t="s">
+      <c r="N5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="17" t="s">
+      <c r="G6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="18" t="s">
+      <c r="L6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="O6" s="18" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1361,43 +1479,43 @@
       <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="17" t="s">
+      <c r="D7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="17" t="s">
+      <c r="H7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="O7" s="22" t="s">
+      <c r="N7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="21" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1412,15 +1530,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R22"/>
+  <dimension ref="B1:R24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G27" sqref="G27"/>
+      <selection pane="topRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,537 +1558,1200 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="O2" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="46"/>
+      <c r="C4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="46"/>
+      <c r="C5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="47"/>
+      <c r="C6" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q6" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="46"/>
+      <c r="C8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="46"/>
+      <c r="C9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="47"/>
+      <c r="C10" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="P10" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q10" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="R10" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="R11" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="46"/>
+      <c r="C12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="46"/>
+      <c r="C13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="47"/>
+      <c r="C14" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L14" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="P14" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q14" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="R14" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="R15" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="46"/>
+      <c r="C16" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="46"/>
+      <c r="C17" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R17" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="47"/>
+      <c r="C18" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="M18" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q18" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R18" s="29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="R19" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="46"/>
+      <c r="C20" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="P20" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q20" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="R20" s="33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="46"/>
+      <c r="C21" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="R21" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="L22" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="M22" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="N22" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="P22" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="R22" s="52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="58"/>
+      <c r="C23" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="O3" s="48"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="49"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="28"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="15"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="28"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="13"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="33"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36" t="s">
+      <c r="F23" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="I23" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="L23" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="M23" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="36"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="37"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="28"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="15"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="13"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="30"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="33"/>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="N11" s="36"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="37"/>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="15"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="13"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="30"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="33"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="36" t="s">
+      <c r="N23" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="O23" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="P23" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q23" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="R23" s="56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="59"/>
+      <c r="C24" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="N15" s="36"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="37"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="15"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="28"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="13"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="30"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="33"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N19" s="7"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="13"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="28"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="38"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="28"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="13"/>
-    </row>
-    <row r="22" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="29"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="43"/>
+      <c r="G24" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="L24" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="M24" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="P24" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q24" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="R24" s="38" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B22:B24"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B19:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
More TESTINGgit add *
</commit_message>
<xml_diff>
--- a/Lab_2/Report/ControlSignals.xlsx
+++ b/Lab_2/Report/ControlSignals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Data Path B" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="84">
   <si>
     <t>W_EN</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>---------10</t>
+  </si>
+  <si>
+    <t>ØØ1Ø</t>
   </si>
 </sst>
 </file>
@@ -649,6 +652,24 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -661,24 +682,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1236,7 +1239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -1532,9 +1535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G30" sqref="G30"/>
+      <selection pane="topRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,7 +1614,7 @@
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="57" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="39" t="s">
@@ -1642,7 +1645,7 @@
         <v>57</v>
       </c>
       <c r="L3" s="41" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="M3" s="41" t="s">
         <v>29</v>
@@ -1654,7 +1657,7 @@
         <v>22</v>
       </c>
       <c r="P3" s="41" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="41" t="s">
         <v>63</v>
@@ -1664,7 +1667,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="46"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="14" t="s">
         <v>54</v>
       </c>
@@ -1715,7 +1718,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="46"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="12" t="s">
         <v>55</v>
       </c>
@@ -1766,7 +1769,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="47"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="14" t="s">
         <v>56</v>
       </c>
@@ -1817,7 +1820,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="60" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="40" t="s">
@@ -1848,7 +1851,7 @@
         <v>62</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="M7" s="31" t="s">
         <v>29</v>
@@ -1870,7 +1873,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="46"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="14" t="s">
         <v>54</v>
       </c>
@@ -1921,7 +1924,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="46"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="12" t="s">
         <v>55</v>
       </c>
@@ -1972,7 +1975,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="14" t="s">
         <v>56</v>
       </c>
@@ -2023,7 +2026,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="60" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="40" t="s">
@@ -2054,7 +2057,7 @@
         <v>65</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="M11" s="31" t="s">
         <v>29</v>
@@ -2076,7 +2079,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="46"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="14" t="s">
         <v>54</v>
       </c>
@@ -2127,7 +2130,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="46"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="12" t="s">
         <v>55</v>
       </c>
@@ -2178,7 +2181,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="14" t="s">
         <v>56</v>
       </c>
@@ -2229,7 +2232,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="60" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="40" t="s">
@@ -2260,7 +2263,7 @@
         <v>67</v>
       </c>
       <c r="L15" s="31" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="M15" s="31" t="s">
         <v>29</v>
@@ -2282,7 +2285,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="46"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="14" t="s">
         <v>54</v>
       </c>
@@ -2333,7 +2336,7 @@
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="46"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="12" t="s">
         <v>55</v>
       </c>
@@ -2384,7 +2387,7 @@
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="14" t="s">
         <v>69</v>
       </c>
@@ -2435,7 +2438,7 @@
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="58" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="40" t="s">
@@ -2466,7 +2469,7 @@
         <v>70</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>29</v>
@@ -2488,7 +2491,7 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="14" t="s">
         <v>69</v>
       </c>
@@ -2539,7 +2542,7 @@
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="46"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="12" t="s">
         <v>72</v>
       </c>
@@ -2590,112 +2593,112 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="51" t="s">
+      <c r="D22" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" s="51" t="s">
+      <c r="G22" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="L22" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="M22" s="51" t="s">
+      <c r="L22" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="M22" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="N22" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="O22" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="P22" s="51" t="s">
+      <c r="N22" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="P22" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="R22" s="52" t="s">
+      <c r="Q22" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="R22" s="48" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="58"/>
-      <c r="C23" s="53" t="s">
+      <c r="B23" s="55"/>
+      <c r="C23" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="55" t="s">
+      <c r="F23" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="55" t="s">
+      <c r="G23" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="I23" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" s="55" t="s">
+      <c r="I23" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="L23" s="55" t="s">
+      <c r="L23" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="M23" s="55" t="s">
+      <c r="M23" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="N23" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="O23" s="54" t="s">
+      <c r="N23" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="O23" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="P23" s="55" t="s">
+      <c r="P23" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="R23" s="56" t="s">
+      <c r="Q23" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="R23" s="52" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="59"/>
-      <c r="C24" s="60" t="s">
+      <c r="B24" s="56"/>
+      <c r="C24" s="53" t="s">
         <v>55</v>
       </c>
       <c r="D24" s="36" t="s">

</xml_diff>

<commit_message>
Fixed simulation not being synced to clock correctly
</commit_message>
<xml_diff>
--- a/Lab_2/Report/ControlSignals.xlsx
+++ b/Lab_2/Report/ControlSignals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Path B" sheetId="1" r:id="rId1"/>
@@ -1239,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,9 +1535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L3" sqref="L3"/>
+      <selection pane="topRight" activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,7 +1657,7 @@
         <v>22</v>
       </c>
       <c r="P3" s="41" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="Q3" s="41" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Working towards fixing tests
</commit_message>
<xml_diff>
--- a/Lab_2/Report/ControlSignals.xlsx
+++ b/Lab_2/Report/ControlSignals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="83">
   <si>
     <t>W_EN</t>
   </si>
@@ -163,9 +163,6 @@
     <t>PC[15:0]</t>
   </si>
   <si>
-    <t>SH[4:0]</t>
-  </si>
-  <si>
     <t>PC_plus[15:0]</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
     <t>ØØ0Ø</t>
   </si>
   <si>
-    <t xml:space="preserve"> ØØØØØ</t>
-  </si>
-  <si>
     <t>0100</t>
   </si>
   <si>
@@ -272,6 +266,9 @@
   </si>
   <si>
     <t>ØØ1Ø</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ØØØØ</t>
   </si>
 </sst>
 </file>
@@ -1536,8 +1533,10 @@
   <dimension ref="B1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O30" sqref="O30"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>41</v>
@@ -1598,19 +1597,19 @@
         <v>42</v>
       </c>
       <c r="N2" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="P2" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="Q2" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="R2" s="26" t="s">
         <v>50</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
@@ -1618,7 +1617,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="42" t="s">
         <v>10</v>
@@ -1642,16 +1641,16 @@
         <v>12</v>
       </c>
       <c r="K3" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L3" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M3" s="41" t="s">
         <v>29</v>
       </c>
       <c r="N3" s="41" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="O3" s="42" t="s">
         <v>22</v>
@@ -1660,19 +1659,19 @@
         <v>19</v>
       </c>
       <c r="Q3" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R3" s="43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="58"/>
       <c r="C4" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>10</v>
@@ -1693,7 +1692,7 @@
         <v>10</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>22</v>
@@ -1702,25 +1701,25 @@
         <v>10</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R4" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="58"/>
       <c r="C5" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -1744,16 +1743,16 @@
         <v>10</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>22</v>
@@ -1762,16 +1761,16 @@
         <v>43</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R5" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="59"/>
       <c r="C6" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -1795,7 +1794,7 @@
         <v>10</v>
       </c>
       <c r="K6" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L6" s="28" t="s">
         <v>14</v>
@@ -1804,19 +1803,19 @@
         <v>10</v>
       </c>
       <c r="N6" s="28" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="O6" s="27" t="s">
         <v>22</v>
       </c>
       <c r="P6" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q6" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R6" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
@@ -1824,40 +1823,40 @@
         <v>3</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F7" s="31" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K7" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M7" s="31" t="s">
         <v>29</v>
       </c>
       <c r="N7" s="31" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="O7" s="30" t="s">
         <v>22</v>
@@ -1866,100 +1865,100 @@
         <v>19</v>
       </c>
       <c r="Q7" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R7" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="58"/>
       <c r="C8" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="P8" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="58"/>
       <c r="C9" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>30</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>22</v>
@@ -1968,19 +1967,19 @@
         <v>19</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="59"/>
       <c r="C10" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="28" t="s">
         <v>10</v>
@@ -1995,13 +1994,13 @@
         <v>10</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K10" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L10" s="28" t="s">
         <v>14</v>
@@ -2010,19 +2009,19 @@
         <v>10</v>
       </c>
       <c r="N10" s="28" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="O10" s="27" t="s">
         <v>22</v>
       </c>
       <c r="P10" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R10" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
@@ -2030,7 +2029,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>10</v>
@@ -2054,16 +2053,16 @@
         <v>12</v>
       </c>
       <c r="K11" s="31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M11" s="31" t="s">
         <v>29</v>
       </c>
       <c r="N11" s="31" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="O11" s="30" t="s">
         <v>22</v>
@@ -2072,16 +2071,16 @@
         <v>19</v>
       </c>
       <c r="Q11" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R11" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="58"/>
       <c r="C12" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>9</v>
@@ -2105,34 +2104,34 @@
         <v>12</v>
       </c>
       <c r="K12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L12" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="P12" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R12" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="58"/>
       <c r="C13" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>
@@ -2156,16 +2155,16 @@
         <v>10</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M13" s="7" t="s">
         <v>31</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O13" s="30" t="s">
         <v>22</v>
@@ -2174,16 +2173,16 @@
         <v>19</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R13" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="59"/>
       <c r="C14" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>22</v>
@@ -2207,7 +2206,7 @@
         <v>22</v>
       </c>
       <c r="K14" s="28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L14" s="28" t="s">
         <v>14</v>
@@ -2222,13 +2221,13 @@
         <v>22</v>
       </c>
       <c r="P14" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q14" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R14" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
@@ -2236,7 +2235,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>10</v>
@@ -2260,10 +2259,10 @@
         <v>12</v>
       </c>
       <c r="K15" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L15" s="31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M15" s="31" t="s">
         <v>29</v>
@@ -2278,16 +2277,16 @@
         <v>19</v>
       </c>
       <c r="Q15" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R15" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="58"/>
       <c r="C16" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>21</v>
@@ -2311,7 +2310,7 @@
         <v>12</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>22</v>
@@ -2323,22 +2322,22 @@
         <v>22</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R16" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="58"/>
       <c r="C17" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>10</v>
@@ -2362,10 +2361,10 @@
         <v>12</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M17" s="7" t="s">
         <v>7</v>
@@ -2380,16 +2379,16 @@
         <v>19</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="59"/>
       <c r="C18" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>10</v>
@@ -2413,10 +2412,10 @@
         <v>12</v>
       </c>
       <c r="K18" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L18" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M18" s="28" t="s">
         <v>22</v>
@@ -2428,7 +2427,7 @@
         <v>22</v>
       </c>
       <c r="P18" s="28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q18" s="28" t="s">
         <v>23</v>
@@ -2442,7 +2441,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>10</v>
@@ -2466,10 +2465,10 @@
         <v>10</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>29</v>
@@ -2493,7 +2492,7 @@
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="58"/>
       <c r="C20" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>10</v>
@@ -2511,28 +2510,28 @@
         <v>10</v>
       </c>
       <c r="I20" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="J20" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="K20" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="L20" s="35" t="s">
+      <c r="M20" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="M20" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="N20" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="O20" s="34" t="s">
-        <v>77</v>
-      </c>
       <c r="P20" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q20" s="35" t="s">
         <v>24</v>
@@ -2544,7 +2543,7 @@
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="58"/>
       <c r="C21" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
@@ -2568,10 +2567,10 @@
         <v>10</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M21" s="7" t="s">
         <v>22</v>
@@ -2583,7 +2582,7 @@
         <v>22</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q21" s="7" t="s">
         <v>12</v>
@@ -2594,10 +2593,10 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="46" t="s">
         <v>10</v>
@@ -2621,10 +2620,10 @@
         <v>22</v>
       </c>
       <c r="K22" s="47" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L22" s="47" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M22" s="47" t="s">
         <v>29</v>
@@ -2648,7 +2647,7 @@
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="55"/>
       <c r="C23" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="50" t="s">
         <v>16</v>
@@ -2663,7 +2662,7 @@
         <v>10</v>
       </c>
       <c r="H23" s="51" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I23" s="51" t="s">
         <v>22</v>
@@ -2672,10 +2671,10 @@
         <v>22</v>
       </c>
       <c r="K23" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="L23" s="51" t="s">
         <v>77</v>
-      </c>
-      <c r="L23" s="51" t="s">
-        <v>79</v>
       </c>
       <c r="M23" s="51" t="s">
         <v>30</v>
@@ -2684,7 +2683,7 @@
         <v>22</v>
       </c>
       <c r="O23" s="50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P23" s="51" t="s">
         <v>19</v>
@@ -2699,7 +2698,7 @@
     <row r="24" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="56"/>
       <c r="C24" s="53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="36" t="s">
         <v>10</v>
@@ -2723,10 +2722,10 @@
         <v>12</v>
       </c>
       <c r="K24" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L24" s="37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M24" s="37" t="s">
         <v>30</v>
@@ -2735,10 +2734,10 @@
         <v>22</v>
       </c>
       <c r="O24" s="36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P24" s="37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q24" s="37" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Giving up on this for now, Going to get DP_D working
</commit_message>
<xml_diff>
--- a/Lab_2/Report/ControlSignals.xlsx
+++ b/Lab_2/Report/ControlSignals.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data Path B" sheetId="1" r:id="rId1"/>
     <sheet name="Data Path C" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Path D" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -259,9 +260,6 @@
     <t>0105</t>
   </si>
   <si>
-    <t>0214</t>
-  </si>
-  <si>
     <t>---------10</t>
   </si>
   <si>
@@ -269,6 +267,9 @@
   </si>
   <si>
     <t xml:space="preserve"> ØØØØ</t>
+  </si>
+  <si>
+    <t>0213</t>
   </si>
 </sst>
 </file>
@@ -1532,11 +1533,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomRight" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,13 +1645,13 @@
         <v>56</v>
       </c>
       <c r="L3" s="41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M3" s="41" t="s">
         <v>29</v>
       </c>
       <c r="N3" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O3" s="42" t="s">
         <v>22</v>
@@ -1850,7 +1851,7 @@
         <v>60</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M7" s="31" t="s">
         <v>29</v>
@@ -2056,7 +2057,7 @@
         <v>63</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M11" s="31" t="s">
         <v>29</v>
@@ -2262,7 +2263,7 @@
         <v>65</v>
       </c>
       <c r="L15" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M15" s="31" t="s">
         <v>29</v>
@@ -2468,7 +2469,7 @@
         <v>68</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>29</v>
@@ -2623,7 +2624,7 @@
         <v>75</v>
       </c>
       <c r="L22" s="47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M22" s="47" t="s">
         <v>29</v>
@@ -2734,10 +2735,10 @@
         <v>22</v>
       </c>
       <c r="O24" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="P24" s="37" t="s">
         <v>79</v>
-      </c>
-      <c r="P24" s="37" t="s">
-        <v>80</v>
       </c>
       <c r="Q24" s="37" t="s">
         <v>12</v>
@@ -2758,4 +2759,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Realised regbank is broken
</commit_message>
<xml_diff>
--- a/Lab_2/Report/ControlSignals.xlsx
+++ b/Lab_2/Report/ControlSignals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Data Path B" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Data Path D" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="108">
   <si>
     <t>W_EN</t>
   </si>
@@ -270,6 +271,81 @@
   </si>
   <si>
     <t>0213</t>
+  </si>
+  <si>
+    <t>SEL(3)[4]</t>
+  </si>
+  <si>
+    <t>SEL(1)[1:0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEL (4)[5] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEL (5)[6] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEL (6)[7] </t>
+  </si>
+  <si>
+    <t>SEL(2)[3:2]</t>
+  </si>
+  <si>
+    <t>ALU+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fetch</t>
+  </si>
+  <si>
+    <t>Reg Write</t>
+  </si>
+  <si>
+    <t>Reg Read</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>RB</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>IMM</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>M_in</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>nop</t>
+  </si>
+  <si>
+    <t>Ø</t>
+  </si>
+  <si>
+    <t>ØØ</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>0xØØØ</t>
   </si>
 </sst>
 </file>
@@ -306,7 +382,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,8 +407,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB889DB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -600,11 +712,175 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -680,6 +956,96 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,6 +1289,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFB889DB"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1237,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,10 +1906,7 @@
   <dimension ref="B1:R24"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O24" sqref="O24"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2763,12 +3132,952 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="5" width="10" customWidth="1"/>
+    <col min="6" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="11" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="81"/>
+      <c r="C2" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="72"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="76"/>
+    </row>
+    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="62"/>
+      <c r="D3" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="K3" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P3" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q3" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="78" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="86"/>
+      <c r="D4" s="87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="86" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="J4" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="87" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="86" t="s">
+        <v>102</v>
+      </c>
+      <c r="P4" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="88" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="89" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="90"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="90" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="90" t="s">
+        <v>102</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="79" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="90"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="90"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="15"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="90"/>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="90" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="90" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7" s="90" t="s">
+        <v>102</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="90"/>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="L8" s="90" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="O8" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="91"/>
+      <c r="D9" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="93" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="91" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="92" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="93" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="93" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="L9" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="92" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="93" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="93" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" s="94" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="96" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="98" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="96" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="98" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="83"/>
+    </row>
+    <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="82"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="83"/>
+    </row>
+    <row r="18" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="96" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="98" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="83"/>
+    </row>
+    <row r="19" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="96" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" s="98" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19" s="83"/>
+    </row>
+    <row r="20" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="99" t="s">
+        <v>90</v>
+      </c>
+      <c r="I20" s="100" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="101" t="s">
+        <v>89</v>
+      </c>
+      <c r="K20" s="102" t="s">
+        <v>67</v>
+      </c>
+      <c r="L20" s="103" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="81"/>
+      <c r="C24" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="70"/>
+      <c r="M24" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="N24" s="72"/>
+      <c r="O24" s="73"/>
+      <c r="P24" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q24" s="75"/>
+      <c r="R24" s="76"/>
+    </row>
+    <row r="25" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="62"/>
+      <c r="D25" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="J25" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="K25" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="L25" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="M25" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="N25" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="O25" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P25" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q25" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="R25" s="78" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="111">
+        <v>1</v>
+      </c>
+      <c r="C26" s="116"/>
+      <c r="D26" s="117" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="116" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="116" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="118" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" s="119"/>
+      <c r="I26" s="119"/>
+      <c r="J26" s="119"/>
+      <c r="K26" s="119"/>
+      <c r="L26" s="119"/>
+      <c r="M26" s="120"/>
+      <c r="N26" s="119"/>
+      <c r="O26" s="121"/>
+      <c r="P26" s="119"/>
+      <c r="Q26" s="119"/>
+      <c r="R26" s="122"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="104">
+        <v>2</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="106" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="I27" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="J27" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="K27" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" s="108"/>
+      <c r="N27" s="107"/>
+      <c r="O27" s="109"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="110"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="104">
+        <v>3</v>
+      </c>
+      <c r="C28" s="35"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="106"/>
+      <c r="H28" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="I28" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="J28" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N28" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="O28" s="106" t="s">
+        <v>102</v>
+      </c>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="110"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="104">
+        <v>4</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G29" s="106" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N29" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="106" t="s">
+        <v>102</v>
+      </c>
+      <c r="P29" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="R29" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="104">
+        <v>5</v>
+      </c>
+      <c r="C30" s="35"/>
+      <c r="D30" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="I30" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="J30" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="K30" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="34"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="106"/>
+      <c r="P30" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q30" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="R30" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="104">
+        <v>6</v>
+      </c>
+      <c r="C31" s="35"/>
+      <c r="D31" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" s="106" t="s">
+        <v>102</v>
+      </c>
+      <c r="H31" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="I31" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="J31" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="L31" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="M31" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="N31" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="O31" s="106" t="s">
+        <v>102</v>
+      </c>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="33"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="104">
+        <v>7</v>
+      </c>
+      <c r="C32" s="35"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="106"/>
+      <c r="H32" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="I32" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="J32" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="L32" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="M32" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="N32" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="O32" s="106" t="s">
+        <v>11</v>
+      </c>
+      <c r="P32" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q32" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="R32" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B33" s="104">
+        <v>8</v>
+      </c>
+      <c r="C33" s="35"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="N33" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="O33" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="P33" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q33" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="R33" s="33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="105">
+        <v>9</v>
+      </c>
+      <c r="C34" s="112"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="114"/>
+      <c r="H34" s="112"/>
+      <c r="I34" s="112"/>
+      <c r="J34" s="112"/>
+      <c r="K34" s="112"/>
+      <c r="L34" s="112"/>
+      <c r="M34" s="113"/>
+      <c r="N34" s="112"/>
+      <c r="O34" s="114"/>
+      <c r="P34" s="112" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q34" s="112" t="s">
+        <v>15</v>
+      </c>
+      <c r="R34" s="115" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="H24:L24"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
B and C working git status!
</commit_message>
<xml_diff>
--- a/Lab_2/Report/ControlSignals.xlsx
+++ b/Lab_2/Report/ControlSignals.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Data Path D" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="109">
   <si>
     <t>W_EN</t>
   </si>
@@ -346,13 +345,16 @@
   </si>
   <si>
     <t>0xØØØ</t>
+  </si>
+  <si>
+    <t>OEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +382,11 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
     </font>
   </fonts>
   <fills count="11">
@@ -880,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -935,67 +942,10 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1046,11 +996,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1307,8 +1330,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:O7" totalsRowShown="0" tableBorderDxfId="14">
-  <autoFilter ref="B2:O7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:P7" totalsRowShown="0" tableBorderDxfId="15">
+  <autoFilter ref="B2:P7">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1324,21 +1347,22 @@
     <filterColumn colId="12" hiddenButton="1"/>
     <filterColumn colId="13" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="14">
-    <tableColumn id="1" name="Test Command" dataDxfId="13"/>
-    <tableColumn id="2" name="W_EN" dataDxfId="12"/>
-    <tableColumn id="3" name="AL[3:0]" dataDxfId="11"/>
-    <tableColumn id="4" name="R_A[4:0]" dataDxfId="10"/>
-    <tableColumn id="5" name="R_B[4:0]" dataDxfId="9"/>
-    <tableColumn id="6" name="W_A[4:0]" dataDxfId="8"/>
-    <tableColumn id="7" name="IMM[15:0]" dataDxfId="7"/>
-    <tableColumn id="8" name="SH[3:0]" dataDxfId="6"/>
-    <tableColumn id="9" name="M_A[3:0]" dataDxfId="5"/>
-    <tableColumn id="10" name="S[4:1]" dataDxfId="4"/>
-    <tableColumn id="11" name="M_in[3:0]" dataDxfId="3"/>
-    <tableColumn id="12" name="flags[7:0]" dataDxfId="2"/>
-    <tableColumn id="13" name="M_B[3:0]" dataDxfId="1"/>
-    <tableColumn id="14" name="M_DA[3:0]" dataDxfId="0"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="Test Command" dataDxfId="14"/>
+    <tableColumn id="2" name="W_EN" dataDxfId="13"/>
+    <tableColumn id="3" name="AL[3:0]" dataDxfId="12"/>
+    <tableColumn id="4" name="R_A[4:0]" dataDxfId="11"/>
+    <tableColumn id="5" name="R_B[4:0]" dataDxfId="10"/>
+    <tableColumn id="6" name="W_A[4:0]" dataDxfId="9"/>
+    <tableColumn id="7" name="IMM[15:0]" dataDxfId="8"/>
+    <tableColumn id="8" name="SH[3:0]" dataDxfId="7"/>
+    <tableColumn id="9" name="M_A[3:0]" dataDxfId="6"/>
+    <tableColumn id="10" name="S[4:1]" dataDxfId="5"/>
+    <tableColumn id="11" name="M_in[3:0]" dataDxfId="4"/>
+    <tableColumn id="12" name="flags[7:0]" dataDxfId="3"/>
+    <tableColumn id="13" name="M_B[3:0]" dataDxfId="2"/>
+    <tableColumn id="14" name="M_DA[3:0]" dataDxfId="1"/>
+    <tableColumn id="15" name="OEN" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1607,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,8 +1648,8 @@
     <col min="15" max="15" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1668,8 +1692,11 @@
       <c r="O2" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
@@ -1712,8 +1739,11 @@
       <c r="O3" s="18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
       <c r="B4" s="10" t="s">
         <v>3</v>
@@ -1757,8 +1787,11 @@
       <c r="O4" s="18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="124" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="10" t="s">
         <v>4</v>
@@ -1802,8 +1835,11 @@
       <c r="O5" s="18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="124" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="10" t="s">
         <v>5</v>
@@ -1847,8 +1883,11 @@
       <c r="O6" s="18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="124" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
@@ -1890,6 +1929,9 @@
       </c>
       <c r="O7" s="21" t="s">
         <v>24</v>
+      </c>
+      <c r="P7" s="124" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1903,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R24"/>
+  <dimension ref="B1:S24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,8 +1970,8 @@
     <col min="18" max="18" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="44" t="s">
         <v>1</v>
       </c>
@@ -1981,9 +2023,12 @@
       <c r="R2" s="26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="57" t="s">
+      <c r="S2" s="123" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="107" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="39" t="s">
@@ -2034,9 +2079,12 @@
       <c r="R3" s="43" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="58"/>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="108"/>
       <c r="C4" s="14" t="s">
         <v>53</v>
       </c>
@@ -2085,9 +2133,12 @@
       <c r="R4" s="15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="58"/>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="108"/>
       <c r="C5" s="12" t="s">
         <v>54</v>
       </c>
@@ -2136,9 +2187,12 @@
       <c r="R5" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="59"/>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="109"/>
       <c r="C6" s="14" t="s">
         <v>55</v>
       </c>
@@ -2187,9 +2241,12 @@
       <c r="R6" s="29" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="60" t="s">
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="110" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="40" t="s">
@@ -2240,9 +2297,12 @@
       <c r="R7" s="32" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="58"/>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="108"/>
       <c r="C8" s="14" t="s">
         <v>53</v>
       </c>
@@ -2291,9 +2351,12 @@
       <c r="R8" s="15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="108"/>
       <c r="C9" s="12" t="s">
         <v>54</v>
       </c>
@@ -2342,9 +2405,12 @@
       <c r="R9" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="59"/>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="109"/>
       <c r="C10" s="14" t="s">
         <v>55</v>
       </c>
@@ -2393,9 +2459,12 @@
       <c r="R10" s="29" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="60" t="s">
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="110" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="40" t="s">
@@ -2446,9 +2515,12 @@
       <c r="R11" s="32" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="58"/>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="108"/>
       <c r="C12" s="14" t="s">
         <v>53</v>
       </c>
@@ -2497,9 +2569,12 @@
       <c r="R12" s="15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="108"/>
       <c r="C13" s="12" t="s">
         <v>54</v>
       </c>
@@ -2548,9 +2623,12 @@
       <c r="R13" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="59"/>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="109"/>
       <c r="C14" s="14" t="s">
         <v>55</v>
       </c>
@@ -2599,9 +2677,12 @@
       <c r="R14" s="29" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="60" t="s">
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="110" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="40" t="s">
@@ -2652,9 +2733,12 @@
       <c r="R15" s="32" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="58"/>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="108"/>
       <c r="C16" s="14" t="s">
         <v>53</v>
       </c>
@@ -2662,7 +2746,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>11</v>
@@ -2703,9 +2787,12 @@
       <c r="R16" s="15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="58"/>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="108"/>
       <c r="C17" s="12" t="s">
         <v>54</v>
       </c>
@@ -2713,7 +2800,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>11</v>
@@ -2754,9 +2841,12 @@
       <c r="R17" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="59"/>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="109"/>
       <c r="C18" s="14" t="s">
         <v>67</v>
       </c>
@@ -2805,9 +2895,12 @@
       <c r="R18" s="29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="58" t="s">
+      <c r="S18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="108" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="40" t="s">
@@ -2858,9 +2951,12 @@
       <c r="R19" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="58"/>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="108"/>
       <c r="C20" s="14" t="s">
         <v>67</v>
       </c>
@@ -2909,9 +3005,12 @@
       <c r="R20" s="33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="58"/>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="108"/>
       <c r="C21" s="12" t="s">
         <v>70</v>
       </c>
@@ -2960,9 +3059,12 @@
       <c r="R21" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="54" t="s">
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="104" t="s">
         <v>69</v>
       </c>
       <c r="C22" s="45" t="s">
@@ -3013,9 +3115,12 @@
       <c r="R22" s="48" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="55"/>
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="105"/>
       <c r="C23" s="49" t="s">
         <v>53</v>
       </c>
@@ -3064,9 +3169,12 @@
       <c r="R23" s="52" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="56"/>
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="106"/>
       <c r="C24" s="53" t="s">
         <v>54</v>
       </c>
@@ -3114,6 +3222,9 @@
       </c>
       <c r="R24" s="38" t="s">
         <v>12</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3152,141 +3263,141 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="81"/>
-      <c r="C2" s="64" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68" t="s">
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="120" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="71" t="s">
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="72"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="74" t="s">
+      <c r="N2" s="112"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="114" t="s">
         <v>91</v>
       </c>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="76"/>
+      <c r="Q2" s="115"/>
+      <c r="R2" s="116"/>
     </row>
     <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="63" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="63" t="s">
+      <c r="H3" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="61" t="s">
+      <c r="I3" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="61" t="s">
+      <c r="J3" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="61" t="s">
+      <c r="K3" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="62" t="s">
+      <c r="L3" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="63" t="s">
+      <c r="M3" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="61" t="s">
+      <c r="N3" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="O3" s="62" t="s">
+      <c r="O3" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="P3" s="63" t="s">
+      <c r="P3" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="Q3" s="61" t="s">
+      <c r="Q3" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="78" t="s">
+      <c r="R3" s="59" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="87" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="88" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="88" t="s">
+      <c r="E4" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="86" t="s">
+      <c r="G4" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="87" t="s">
+      <c r="H4" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="88" t="s">
+      <c r="I4" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="J4" s="88" t="s">
+      <c r="J4" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="86" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="86" t="s">
+      <c r="K4" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="P4" s="87" t="s">
+      <c r="P4" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="88" t="s">
+      <c r="Q4" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="89" t="s">
+      <c r="R4" s="70" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="90"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
@@ -3296,7 +3407,7 @@
       <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="90" t="s">
+      <c r="G5" s="71" t="s">
         <v>102</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -3311,7 +3422,7 @@
       <c r="K5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="90" t="s">
+      <c r="L5" s="71" t="s">
         <v>10</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -3320,7 +3431,7 @@
       <c r="N5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="90" t="s">
+      <c r="O5" s="71" t="s">
         <v>102</v>
       </c>
       <c r="P5" s="2" t="s">
@@ -3334,31 +3445,31 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="90"/>
+      <c r="C6" s="71"/>
       <c r="D6" s="2"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="90"/>
+      <c r="G6" s="71"/>
       <c r="H6" s="2"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="L6" s="90"/>
+      <c r="L6" s="71"/>
       <c r="M6" s="2"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="90"/>
+      <c r="O6" s="71"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="15"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="90"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3368,7 +3479,7 @@
       <c r="F7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="90" t="s">
+      <c r="G7" s="71" t="s">
         <v>102</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -3383,7 +3494,7 @@
       <c r="K7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="90" t="s">
+      <c r="L7" s="71" t="s">
         <v>21</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -3392,7 +3503,7 @@
       <c r="N7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="O7" s="90" t="s">
+      <c r="O7" s="71" t="s">
         <v>102</v>
       </c>
       <c r="P7" s="2" t="s">
@@ -3406,10 +3517,10 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="79" t="s">
+      <c r="B8" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="90"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
@@ -3419,7 +3530,7 @@
       <c r="F8" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G8" s="90" t="s">
+      <c r="G8" s="71" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -3434,7 +3545,7 @@
       <c r="K8" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="L8" s="90" t="s">
+      <c r="L8" s="71" t="s">
         <v>22</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -3443,7 +3554,7 @@
       <c r="N8" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="O8" s="90" t="s">
+      <c r="O8" s="71" t="s">
         <v>11</v>
       </c>
       <c r="P8" s="2" t="s">
@@ -3457,53 +3568,53 @@
       </c>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="92" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="93" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="93" t="s">
+      <c r="C9" s="72"/>
+      <c r="D9" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="G9" s="91" t="s">
+      <c r="G9" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="H9" s="92" t="s">
+      <c r="H9" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="I9" s="93" t="s">
+      <c r="I9" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="J9" s="93" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="93" t="s">
+      <c r="J9" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="L9" s="91" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="92" t="s">
+      <c r="L9" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="93" t="s">
+      <c r="N9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="91" t="s">
+      <c r="O9" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="P9" s="92" t="s">
+      <c r="P9" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="Q9" s="93" t="s">
+      <c r="Q9" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="R9" s="94" t="s">
+      <c r="R9" s="75" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3512,19 +3623,19 @@
       <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="96" t="s">
+      <c r="E15" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="97" t="s">
+      <c r="F15" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="98" t="s">
+      <c r="G15" s="79" t="s">
         <v>91</v>
       </c>
       <c r="H15" s="5"/>
@@ -3534,32 +3645,32 @@
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="63" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="95" t="s">
+      <c r="E16" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="96" t="s">
+      <c r="F16" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="97" t="s">
+      <c r="G16" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="98" t="s">
+      <c r="H16" s="79" t="s">
         <v>91</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="83"/>
+      <c r="L16" s="64"/>
     </row>
     <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="82"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -3569,195 +3680,195 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="83"/>
+      <c r="L17" s="64"/>
     </row>
     <row r="18" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="63" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="95" t="s">
+      <c r="G18" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="H18" s="96" t="s">
+      <c r="H18" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="I18" s="97" t="s">
+      <c r="I18" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="98" t="s">
+      <c r="J18" s="79" t="s">
         <v>91</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18" s="83"/>
+      <c r="L18" s="64"/>
     </row>
     <row r="19" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="63" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="64" t="s">
+      <c r="G19" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="95" t="s">
+      <c r="H19" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="96" t="s">
+      <c r="I19" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="J19" s="97" t="s">
+      <c r="J19" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="K19" s="98" t="s">
+      <c r="K19" s="79" t="s">
         <v>91</v>
       </c>
-      <c r="L19" s="83"/>
+      <c r="L19" s="64"/>
     </row>
     <row r="20" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="99" t="s">
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="I20" s="100" t="s">
+      <c r="I20" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="J20" s="101" t="s">
+      <c r="J20" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="K20" s="102" t="s">
+      <c r="K20" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="L20" s="103" t="s">
+      <c r="L20" s="84" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="81"/>
-      <c r="C24" s="64" t="s">
+      <c r="B24" s="62"/>
+      <c r="C24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="65" t="s">
+      <c r="D24" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="68" t="s">
+      <c r="E24" s="118"/>
+      <c r="F24" s="118"/>
+      <c r="G24" s="119"/>
+      <c r="H24" s="120" t="s">
         <v>89</v>
       </c>
-      <c r="I24" s="69"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="70"/>
-      <c r="M24" s="71" t="s">
+      <c r="I24" s="121"/>
+      <c r="J24" s="121"/>
+      <c r="K24" s="121"/>
+      <c r="L24" s="122"/>
+      <c r="M24" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="N24" s="72"/>
-      <c r="O24" s="73"/>
-      <c r="P24" s="74" t="s">
+      <c r="N24" s="112"/>
+      <c r="O24" s="113"/>
+      <c r="P24" s="114" t="s">
         <v>91</v>
       </c>
-      <c r="Q24" s="75"/>
-      <c r="R24" s="76"/>
+      <c r="Q24" s="115"/>
+      <c r="R24" s="116"/>
     </row>
     <row r="25" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="77" t="s">
+      <c r="B25" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="63" t="s">
+      <c r="C25" s="55"/>
+      <c r="D25" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="61" t="s">
+      <c r="E25" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="61" t="s">
+      <c r="F25" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="62" t="s">
+      <c r="G25" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="H25" s="63" t="s">
+      <c r="H25" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="I25" s="61" t="s">
+      <c r="I25" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="J25" s="61" t="s">
+      <c r="J25" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="K25" s="61" t="s">
+      <c r="K25" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="L25" s="62" t="s">
+      <c r="L25" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="M25" s="63" t="s">
+      <c r="M25" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="N25" s="61" t="s">
+      <c r="N25" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="O25" s="62" t="s">
+      <c r="O25" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="P25" s="63" t="s">
+      <c r="P25" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="Q25" s="61" t="s">
+      <c r="Q25" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="R25" s="78" t="s">
+      <c r="R25" s="59" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="111">
+      <c r="B26" s="92">
         <v>1</v>
       </c>
-      <c r="C26" s="116"/>
-      <c r="D26" s="117" t="s">
+      <c r="C26" s="97"/>
+      <c r="D26" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="116" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="116" t="s">
+      <c r="E26" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="118" t="s">
+      <c r="G26" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="H26" s="119"/>
-      <c r="I26" s="119"/>
-      <c r="J26" s="119"/>
-      <c r="K26" s="119"/>
-      <c r="L26" s="119"/>
-      <c r="M26" s="120"/>
-      <c r="N26" s="119"/>
-      <c r="O26" s="121"/>
-      <c r="P26" s="119"/>
-      <c r="Q26" s="119"/>
-      <c r="R26" s="122"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="100"/>
+      <c r="M26" s="101"/>
+      <c r="N26" s="100"/>
+      <c r="O26" s="102"/>
+      <c r="P26" s="100"/>
+      <c r="Q26" s="100"/>
+      <c r="R26" s="103"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="104">
+      <c r="B27" s="85">
         <v>2</v>
       </c>
       <c r="C27" s="35"/>
@@ -3770,7 +3881,7 @@
       <c r="F27" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="106" t="s">
+      <c r="G27" s="87" t="s">
         <v>102</v>
       </c>
       <c r="H27" s="35" t="s">
@@ -3788,22 +3899,22 @@
       <c r="L27" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="M27" s="108"/>
-      <c r="N27" s="107"/>
-      <c r="O27" s="109"/>
-      <c r="P27" s="107"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="110"/>
+      <c r="M27" s="89"/>
+      <c r="N27" s="88"/>
+      <c r="O27" s="90"/>
+      <c r="P27" s="88"/>
+      <c r="Q27" s="88"/>
+      <c r="R27" s="91"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="104">
+      <c r="B28" s="85">
         <v>3</v>
       </c>
       <c r="C28" s="35"/>
       <c r="D28" s="34"/>
       <c r="E28" s="35"/>
       <c r="F28" s="35"/>
-      <c r="G28" s="106"/>
+      <c r="G28" s="87"/>
       <c r="H28" s="35" t="s">
         <v>104</v>
       </c>
@@ -3825,15 +3936,15 @@
       <c r="N28" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O28" s="106" t="s">
+      <c r="O28" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="110"/>
+      <c r="P28" s="88"/>
+      <c r="Q28" s="88"/>
+      <c r="R28" s="91"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="104">
+      <c r="B29" s="85">
         <v>4</v>
       </c>
       <c r="C29" s="35"/>
@@ -3846,7 +3957,7 @@
       <c r="F29" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="G29" s="106" t="s">
+      <c r="G29" s="87" t="s">
         <v>102</v>
       </c>
       <c r="H29" s="35"/>
@@ -3860,7 +3971,7 @@
       <c r="N29" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="O29" s="106" t="s">
+      <c r="O29" s="87" t="s">
         <v>102</v>
       </c>
       <c r="P29" s="35" t="s">
@@ -3874,7 +3985,7 @@
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B30" s="104">
+      <c r="B30" s="85">
         <v>5</v>
       </c>
       <c r="C30" s="35"/>
@@ -3887,7 +3998,7 @@
       <c r="F30" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="G30" s="106" t="s">
+      <c r="G30" s="87" t="s">
         <v>15</v>
       </c>
       <c r="H30" s="35" t="s">
@@ -3907,7 +4018,7 @@
       </c>
       <c r="M30" s="34"/>
       <c r="N30" s="35"/>
-      <c r="O30" s="106"/>
+      <c r="O30" s="87"/>
       <c r="P30" s="35" t="s">
         <v>16</v>
       </c>
@@ -3919,7 +4030,7 @@
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="104">
+      <c r="B31" s="85">
         <v>6</v>
       </c>
       <c r="C31" s="35"/>
@@ -3932,7 +4043,7 @@
       <c r="F31" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="G31" s="106" t="s">
+      <c r="G31" s="87" t="s">
         <v>102</v>
       </c>
       <c r="H31" s="35" t="s">
@@ -3956,7 +4067,7 @@
       <c r="N31" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="O31" s="106" t="s">
+      <c r="O31" s="87" t="s">
         <v>102</v>
       </c>
       <c r="P31" s="35"/>
@@ -3964,14 +4075,14 @@
       <c r="R31" s="33"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="104">
+      <c r="B32" s="85">
         <v>7</v>
       </c>
       <c r="C32" s="35"/>
       <c r="D32" s="34"/>
       <c r="E32" s="35"/>
       <c r="F32" s="35"/>
-      <c r="G32" s="106"/>
+      <c r="G32" s="87"/>
       <c r="H32" s="35" t="s">
         <v>103</v>
       </c>
@@ -3993,7 +4104,7 @@
       <c r="N32" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="O32" s="106" t="s">
+      <c r="O32" s="87" t="s">
         <v>11</v>
       </c>
       <c r="P32" s="35" t="s">
@@ -4007,14 +4118,14 @@
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B33" s="104">
+      <c r="B33" s="85">
         <v>8</v>
       </c>
       <c r="C33" s="35"/>
       <c r="D33" s="34"/>
       <c r="E33" s="35"/>
       <c r="F33" s="35"/>
-      <c r="G33" s="106"/>
+      <c r="G33" s="87"/>
       <c r="H33" s="35"/>
       <c r="I33" s="35"/>
       <c r="J33" s="35"/>
@@ -4026,7 +4137,7 @@
       <c r="N33" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="O33" s="106" t="s">
+      <c r="O33" s="87" t="s">
         <v>15</v>
       </c>
       <c r="P33" s="35" t="s">
@@ -4040,29 +4151,29 @@
       </c>
     </row>
     <row r="34" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="105">
+      <c r="B34" s="86">
         <v>9</v>
       </c>
-      <c r="C34" s="112"/>
-      <c r="D34" s="113"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="114"/>
-      <c r="H34" s="112"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="112"/>
-      <c r="K34" s="112"/>
-      <c r="L34" s="112"/>
-      <c r="M34" s="113"/>
-      <c r="N34" s="112"/>
-      <c r="O34" s="114"/>
-      <c r="P34" s="112" t="s">
+      <c r="C34" s="93"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="93"/>
+      <c r="J34" s="93"/>
+      <c r="K34" s="93"/>
+      <c r="L34" s="93"/>
+      <c r="M34" s="94"/>
+      <c r="N34" s="93"/>
+      <c r="O34" s="95"/>
+      <c r="P34" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="Q34" s="112" t="s">
+      <c r="Q34" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="R34" s="115" t="s">
+      <c r="R34" s="96" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Figured out outputs for Arch D
</commit_message>
<xml_diff>
--- a/Lab_2/Report/ControlSignals.xlsx
+++ b/Lab_2/Report/ControlSignals.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="116">
   <si>
     <t>W_EN</t>
   </si>
@@ -348,6 +348,27 @@
   </si>
   <si>
     <t>OEN</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
+  <si>
+    <t>M_DA</t>
+  </si>
+  <si>
+    <t>M_out</t>
+  </si>
+  <si>
+    <t>Clock cycle</t>
+  </si>
+  <si>
+    <t>Test command</t>
+  </si>
+  <si>
+    <t>TimeLine</t>
+  </si>
+  <si>
+    <t>Empty space should be treated as "don’t care" Ø</t>
   </si>
 </sst>
 </file>
@@ -446,12 +467,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -721,9 +742,22 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -734,75 +768,7 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -869,13 +835,135 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -887,7 +975,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -942,60 +1030,17 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1025,7 +1070,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1043,7 +1088,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1052,9 +1097,82 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1739,7 +1857,7 @@
       <c r="O3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="105">
+      <c r="P3" s="64">
         <v>0</v>
       </c>
     </row>
@@ -1787,7 +1905,7 @@
       <c r="O4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="105" t="s">
+      <c r="P4" s="64" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1835,7 +1953,7 @@
       <c r="O5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="105" t="s">
+      <c r="P5" s="64" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1883,7 +2001,7 @@
       <c r="O6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="105" t="s">
+      <c r="P6" s="64" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1930,7 +2048,7 @@
       <c r="O7" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="P7" s="105" t="s">
+      <c r="P7" s="64" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2023,12 +2141,12 @@
       <c r="R2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="S2" s="104" t="s">
+      <c r="S2" s="63" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="68" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="39" t="s">
@@ -2084,7 +2202,7 @@
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="110"/>
+      <c r="B4" s="69"/>
       <c r="C4" s="14" t="s">
         <v>53</v>
       </c>
@@ -2138,7 +2256,7 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="110"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="12" t="s">
         <v>54</v>
       </c>
@@ -2192,7 +2310,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="111"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="14" t="s">
         <v>55</v>
       </c>
@@ -2246,7 +2364,7 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="71" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="40" t="s">
@@ -2302,7 +2420,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="110"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="14" t="s">
         <v>53</v>
       </c>
@@ -2356,7 +2474,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="110"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="12" t="s">
         <v>54</v>
       </c>
@@ -2410,7 +2528,7 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="111"/>
+      <c r="B10" s="70"/>
       <c r="C10" s="14" t="s">
         <v>55</v>
       </c>
@@ -2464,7 +2582,7 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="71" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="40" t="s">
@@ -2520,7 +2638,7 @@
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="110"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="14" t="s">
         <v>53</v>
       </c>
@@ -2574,7 +2692,7 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="110"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="12" t="s">
         <v>54</v>
       </c>
@@ -2628,7 +2746,7 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="111"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="14" t="s">
         <v>55</v>
       </c>
@@ -2682,7 +2800,7 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="112" t="s">
+      <c r="B15" s="71" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="40" t="s">
@@ -2738,7 +2856,7 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="110"/>
+      <c r="B16" s="69"/>
       <c r="C16" s="14" t="s">
         <v>53</v>
       </c>
@@ -2792,7 +2910,7 @@
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="110"/>
+      <c r="B17" s="69"/>
       <c r="C17" s="12" t="s">
         <v>54</v>
       </c>
@@ -2846,7 +2964,7 @@
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="111"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="14" t="s">
         <v>67</v>
       </c>
@@ -2900,7 +3018,7 @@
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="110" t="s">
+      <c r="B19" s="69" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="40" t="s">
@@ -2956,7 +3074,7 @@
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="110"/>
+      <c r="B20" s="69"/>
       <c r="C20" s="14" t="s">
         <v>67</v>
       </c>
@@ -3010,7 +3128,7 @@
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="110"/>
+      <c r="B21" s="69"/>
       <c r="C21" s="12" t="s">
         <v>70</v>
       </c>
@@ -3064,7 +3182,7 @@
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="106" t="s">
+      <c r="B22" s="65" t="s">
         <v>69</v>
       </c>
       <c r="C22" s="45" t="s">
@@ -3120,7 +3238,7 @@
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="107"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="49" t="s">
         <v>53</v>
       </c>
@@ -3174,7 +3292,7 @@
       </c>
     </row>
     <row r="24" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="108"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="53" t="s">
         <v>54</v>
       </c>
@@ -3243,455 +3361,546 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S34"/>
+  <dimension ref="B1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="5" width="10" customWidth="1"/>
     <col min="6" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="9" width="12.42578125" customWidth="1"/>
     <col min="10" max="11" width="10.42578125" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="14" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="19" width="10.85546875" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="62"/>
-      <c r="C2" s="57" t="s">
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="57"/>
+      <c r="C2" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="119" t="s">
+      <c r="D2" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="122" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="113" t="s">
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="114"/>
-      <c r="O2" s="115"/>
-      <c r="P2" s="116" t="s">
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="118"/>
-    </row>
-    <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="58" t="s">
+      <c r="U2" s="76"/>
+      <c r="V2" s="77"/>
+    </row>
+    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56" t="s">
+      <c r="C3" s="85"/>
+      <c r="D3" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="55" t="s">
+      <c r="G3" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="87" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="55" t="s">
+      <c r="L3" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="M3" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="N3" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="54" t="s">
+      <c r="O3" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="O3" s="55" t="s">
+      <c r="P3" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="P3" s="56" t="s">
+      <c r="Q3" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="R3" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="S3" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="T3" s="86" t="s">
         <v>100</v>
       </c>
-      <c r="Q3" s="54" t="s">
+      <c r="U3" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="59" t="s">
+      <c r="V3" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="S3" s="104" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="58" t="s">
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="68" t="s">
+      <c r="C4" s="114"/>
+      <c r="D4" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="69" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="69" t="s">
+      <c r="E4" s="116" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="67" t="s">
+      <c r="G4" s="114" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="68" t="s">
+      <c r="H4" s="115" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="69" t="s">
+      <c r="I4" s="116" t="s">
         <v>103</v>
       </c>
-      <c r="J4" s="69" t="s">
+      <c r="J4" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="67" t="s">
+      <c r="K4" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="116" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="116" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="116" t="s">
         <v>102</v>
       </c>
-      <c r="P4" s="68" t="s">
+      <c r="Q4" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" s="117">
+        <v>0</v>
+      </c>
+      <c r="T4" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="69" t="s">
+      <c r="U4" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="70" t="s">
+      <c r="V4" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="S4">
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="119"/>
+      <c r="D5" s="120" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="121" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="120" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" s="121" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" s="121" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="121" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="121" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="121" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="120" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q5" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="R5" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="122">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="60" t="s">
+      <c r="T5" s="120" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="121" t="s">
+        <v>15</v>
+      </c>
+      <c r="V5" s="123" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="124"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="126" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="125"/>
+      <c r="O6" s="126"/>
+      <c r="P6" s="126"/>
+      <c r="Q6" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="127">
+        <v>0</v>
+      </c>
+      <c r="T6" s="125"/>
+      <c r="U6" s="126"/>
+      <c r="V6" s="128"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="119"/>
+      <c r="D7" s="120" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="120" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="121" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" s="121" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="121" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="121" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="120" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="P7" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q7" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="R7" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="S7" s="122">
+        <v>0</v>
+      </c>
+      <c r="T7" s="120" t="s">
+        <v>102</v>
+      </c>
+      <c r="U7" s="121" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7" s="123" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="124"/>
+      <c r="D8" s="125" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="126" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="126" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="125" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="126" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="126" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="126" t="s">
+        <v>107</v>
+      </c>
+      <c r="L8" s="126" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="126" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="125" t="s">
+        <v>102</v>
+      </c>
+      <c r="O8" s="126" t="s">
+        <v>102</v>
+      </c>
+      <c r="P8" s="126" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="126" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="126" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" s="127">
+        <v>1</v>
+      </c>
+      <c r="T8" s="125" t="s">
+        <v>102</v>
+      </c>
+      <c r="U8" s="126" t="s">
+        <v>11</v>
+      </c>
+      <c r="V8" s="128" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="129"/>
+      <c r="D9" s="130" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="131" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="131" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="129" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="130" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="131" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="131" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="131" t="s">
+        <v>107</v>
+      </c>
+      <c r="L9" s="131" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="131" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="130" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="131" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="131" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="131" t="s">
+        <v>24</v>
+      </c>
+      <c r="R9" s="131" t="s">
+        <v>12</v>
+      </c>
+      <c r="S9" s="132">
+        <v>0</v>
+      </c>
+      <c r="T9" s="130" t="s">
+        <v>25</v>
+      </c>
+      <c r="U9" s="131" t="s">
+        <v>15</v>
+      </c>
+      <c r="V9" s="133" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="106" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="107" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="107"/>
+      <c r="K14" s="107"/>
+      <c r="L14" s="108"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="102" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="90" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="91" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="92" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="71" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" s="71" t="s">
-        <v>102</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="R5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="15"/>
-      <c r="S6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" s="71" t="s">
-        <v>102</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="71" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="O7" s="71" t="s">
-        <v>102</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="R7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="71" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="L8" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="O8" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="R8" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="61" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="74" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="74" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="72" t="s">
-        <v>102</v>
-      </c>
-      <c r="H9" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="I9" s="74" t="s">
-        <v>103</v>
-      </c>
-      <c r="J9" s="74" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="74" t="s">
-        <v>107</v>
-      </c>
-      <c r="L9" s="72" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="N9" s="74" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="P9" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q9" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="R9" s="75" t="s">
-        <v>11</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="57" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="76" t="s">
+      <c r="E16" s="94" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="F16" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="78" t="s">
+      <c r="G16" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="79" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="57" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="76" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16" s="77" t="s">
-        <v>89</v>
-      </c>
-      <c r="G16" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="79" t="s">
+      <c r="H16" s="97" t="s">
         <v>91</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="64"/>
-    </row>
-    <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="63"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="102" t="s">
+        <v>101</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -3701,543 +3910,622 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="64"/>
-    </row>
-    <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="63" t="s">
+      <c r="L17" s="58"/>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="102" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="57" t="s">
+      <c r="F18" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="76" t="s">
+      <c r="G18" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="H18" s="77" t="s">
+      <c r="H18" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="I18" s="78" t="s">
+      <c r="I18" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="79" t="s">
+      <c r="J18" s="101" t="s">
         <v>91</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18" s="64"/>
-    </row>
-    <row r="19" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="63" t="s">
+      <c r="L18" s="58"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="102" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="57" t="s">
+      <c r="G19" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="76" t="s">
+      <c r="H19" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="77" t="s">
+      <c r="I19" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="J19" s="78" t="s">
+      <c r="J19" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="K19" s="79" t="s">
+      <c r="K19" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="L19" s="64"/>
-    </row>
-    <row r="20" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="65" t="s">
+      <c r="L19" s="58"/>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="80" t="s">
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="109" t="s">
         <v>90</v>
       </c>
-      <c r="I20" s="81" t="s">
+      <c r="I20" s="110" t="s">
         <v>92</v>
       </c>
-      <c r="J20" s="82" t="s">
+      <c r="J20" s="111" t="s">
         <v>89</v>
       </c>
-      <c r="K20" s="83" t="s">
+      <c r="K20" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="L20" s="84" t="s">
+      <c r="L20" s="113" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="62"/>
-      <c r="C24" s="57" t="s">
+    <row r="23" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="57"/>
+      <c r="C24" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="119" t="s">
+      <c r="D24" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="120"/>
-      <c r="F24" s="120"/>
-      <c r="G24" s="121"/>
-      <c r="H24" s="122" t="s">
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="I24" s="123"/>
-      <c r="J24" s="123"/>
-      <c r="K24" s="123"/>
-      <c r="L24" s="124"/>
-      <c r="M24" s="113" t="s">
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="82"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="N24" s="114"/>
-      <c r="O24" s="115"/>
-      <c r="P24" s="116" t="s">
+      <c r="O24" s="73"/>
+      <c r="P24" s="73"/>
+      <c r="Q24" s="73"/>
+      <c r="R24" s="73"/>
+      <c r="S24" s="74"/>
+      <c r="T24" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="Q24" s="117"/>
-      <c r="R24" s="118"/>
-    </row>
-    <row r="25" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="58" t="s">
+      <c r="U24" s="76"/>
+      <c r="V24" s="77"/>
+    </row>
+    <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="85"/>
+      <c r="D25" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="87" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="87" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="85" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="86" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" s="87" t="s">
+        <v>84</v>
+      </c>
+      <c r="J25" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="K25" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="L25" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="M25" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="N25" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="O25" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="P25" s="87" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q25" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="R25" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="S25" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="T25" s="86" t="s">
+        <v>100</v>
+      </c>
+      <c r="U25" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="V25" s="88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="62">
         <v>1</v>
       </c>
-      <c r="C25" s="55"/>
-      <c r="D25" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" s="54" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="H25" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="I25" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="J25" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="K25" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="L25" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="M25" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="N25" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="O25" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="P25" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q25" s="54" t="s">
+      <c r="C26" s="134"/>
+      <c r="D26" s="115" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="116" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="116" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="114" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" s="135"/>
+      <c r="I26" s="135"/>
+      <c r="J26" s="135"/>
+      <c r="K26" s="135"/>
+      <c r="L26" s="135"/>
+      <c r="M26" s="135"/>
+      <c r="N26" s="136"/>
+      <c r="O26" s="117"/>
+      <c r="P26" s="117"/>
+      <c r="Q26" s="117"/>
+      <c r="R26" s="117"/>
+      <c r="S26" s="117">
         <v>0</v>
       </c>
-      <c r="R25" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="S25" s="104" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="92">
+      <c r="T26" s="137"/>
+      <c r="U26" s="135"/>
+      <c r="V26" s="138"/>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="60">
+        <v>2</v>
+      </c>
+      <c r="C27" s="126"/>
+      <c r="D27" s="120" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="121" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="126" t="s">
+        <v>104</v>
+      </c>
+      <c r="I27" s="126" t="s">
+        <v>103</v>
+      </c>
+      <c r="J27" s="126" t="s">
+        <v>29</v>
+      </c>
+      <c r="K27" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="126" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" s="126" t="s">
+        <v>43</v>
+      </c>
+      <c r="N27" s="139"/>
+      <c r="O27" s="122"/>
+      <c r="P27" s="122"/>
+      <c r="Q27" s="122"/>
+      <c r="R27" s="122"/>
+      <c r="S27" s="122">
+        <v>0</v>
+      </c>
+      <c r="T27" s="140"/>
+      <c r="U27" s="127"/>
+      <c r="V27" s="141"/>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B28" s="60">
+        <v>3</v>
+      </c>
+      <c r="C28" s="121"/>
+      <c r="D28" s="125"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="124"/>
+      <c r="H28" s="121" t="s">
+        <v>104</v>
+      </c>
+      <c r="I28" s="121" t="s">
+        <v>105</v>
+      </c>
+      <c r="J28" s="121" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="121" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="121" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="121" t="s">
+        <v>43</v>
+      </c>
+      <c r="N28" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="O28" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="P28" s="126" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q28" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="R28" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="S28" s="127">
+        <v>0</v>
+      </c>
+      <c r="T28" s="139"/>
+      <c r="U28" s="122"/>
+      <c r="V28" s="142"/>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="60">
+        <v>4</v>
+      </c>
+      <c r="C29" s="126"/>
+      <c r="D29" s="120" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="G29" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="126"/>
+      <c r="I29" s="126"/>
+      <c r="J29" s="126"/>
+      <c r="K29" s="126"/>
+      <c r="L29" s="126"/>
+      <c r="M29" s="126"/>
+      <c r="N29" s="120" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="P29" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q29" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="R29" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="S29" s="122">
+        <v>0</v>
+      </c>
+      <c r="T29" s="125" t="s">
+        <v>9</v>
+      </c>
+      <c r="U29" s="126" t="s">
+        <v>15</v>
+      </c>
+      <c r="V29" s="128" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="60">
+        <v>5</v>
+      </c>
+      <c r="C30" s="121"/>
+      <c r="D30" s="125" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="126" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="126" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="121" t="s">
+        <v>106</v>
+      </c>
+      <c r="I30" s="121" t="s">
+        <v>103</v>
+      </c>
+      <c r="J30" s="121" t="s">
+        <v>31</v>
+      </c>
+      <c r="K30" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="121" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="121" t="s">
+        <v>43</v>
+      </c>
+      <c r="N30" s="125"/>
+      <c r="O30" s="126"/>
+      <c r="P30" s="126"/>
+      <c r="Q30" s="126"/>
+      <c r="R30" s="126"/>
+      <c r="S30" s="127">
+        <v>0</v>
+      </c>
+      <c r="T30" s="120" t="s">
+        <v>16</v>
+      </c>
+      <c r="U30" s="121" t="s">
+        <v>15</v>
+      </c>
+      <c r="V30" s="123" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B31" s="60">
+        <v>6</v>
+      </c>
+      <c r="C31" s="126"/>
+      <c r="D31" s="120" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="H31" s="126" t="s">
+        <v>106</v>
+      </c>
+      <c r="I31" s="126" t="s">
+        <v>103</v>
+      </c>
+      <c r="J31" s="126" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="126" t="s">
+        <v>22</v>
+      </c>
+      <c r="M31" s="126" t="s">
+        <v>43</v>
+      </c>
+      <c r="N31" s="120" t="s">
+        <v>12</v>
+      </c>
+      <c r="O31" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="P31" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q31" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="R31" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="S31" s="122">
+        <v>0</v>
+      </c>
+      <c r="T31" s="125"/>
+      <c r="U31" s="126"/>
+      <c r="V31" s="128"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B32" s="60">
+        <v>7</v>
+      </c>
+      <c r="C32" s="121"/>
+      <c r="D32" s="125"/>
+      <c r="E32" s="126"/>
+      <c r="F32" s="126"/>
+      <c r="G32" s="124"/>
+      <c r="H32" s="121" t="s">
+        <v>103</v>
+      </c>
+      <c r="I32" s="121" t="s">
+        <v>103</v>
+      </c>
+      <c r="J32" s="121" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="121" t="s">
+        <v>22</v>
+      </c>
+      <c r="M32" s="121" t="s">
+        <v>28</v>
+      </c>
+      <c r="N32" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" s="126" t="s">
+        <v>102</v>
+      </c>
+      <c r="P32" s="126" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q32" s="126" t="s">
+        <v>23</v>
+      </c>
+      <c r="R32" s="126" t="s">
+        <v>17</v>
+      </c>
+      <c r="S32" s="127">
         <v>1</v>
       </c>
-      <c r="C26" s="97"/>
-      <c r="D26" s="98" t="s">
+      <c r="T32" s="120" t="s">
+        <v>102</v>
+      </c>
+      <c r="U32" s="121" t="s">
+        <v>11</v>
+      </c>
+      <c r="V32" s="123" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="60">
         <v>8</v>
       </c>
-      <c r="E26" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="97" t="s">
+      <c r="C33" s="126"/>
+      <c r="D33" s="120"/>
+      <c r="E33" s="121"/>
+      <c r="F33" s="121"/>
+      <c r="G33" s="119"/>
+      <c r="H33" s="126"/>
+      <c r="I33" s="126"/>
+      <c r="J33" s="126"/>
+      <c r="K33" s="126"/>
+      <c r="L33" s="126"/>
+      <c r="M33" s="126"/>
+      <c r="N33" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="O33" s="121" t="s">
+        <v>27</v>
+      </c>
+      <c r="P33" s="121" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q33" s="121" t="s">
+        <v>24</v>
+      </c>
+      <c r="R33" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="S33" s="122">
+        <v>0</v>
+      </c>
+      <c r="T33" s="125" t="s">
+        <v>102</v>
+      </c>
+      <c r="U33" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="99" t="s">
+      <c r="V33" s="128" t="s">
         <v>102</v>
       </c>
-      <c r="H26" s="100"/>
-      <c r="I26" s="100"/>
-      <c r="J26" s="100"/>
-      <c r="K26" s="100"/>
-      <c r="L26" s="100"/>
-      <c r="M26" s="101"/>
-      <c r="N26" s="100"/>
-      <c r="O26" s="102"/>
-      <c r="P26" s="100"/>
-      <c r="Q26" s="100"/>
-      <c r="R26" s="103"/>
-      <c r="S26">
+    </row>
+    <row r="34" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="61">
+        <v>9</v>
+      </c>
+      <c r="C34" s="131"/>
+      <c r="D34" s="143"/>
+      <c r="E34" s="144"/>
+      <c r="F34" s="144"/>
+      <c r="G34" s="145"/>
+      <c r="H34" s="131"/>
+      <c r="I34" s="131"/>
+      <c r="J34" s="131"/>
+      <c r="K34" s="131"/>
+      <c r="L34" s="131"/>
+      <c r="M34" s="131"/>
+      <c r="N34" s="143"/>
+      <c r="O34" s="144"/>
+      <c r="P34" s="144"/>
+      <c r="Q34" s="144"/>
+      <c r="R34" s="144"/>
+      <c r="S34" s="146">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="85">
-        <v>2</v>
-      </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="35" t="s">
+      <c r="T34" s="130" t="s">
+        <v>25</v>
+      </c>
+      <c r="U34" s="131" t="s">
+        <v>15</v>
+      </c>
+      <c r="V34" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="H27" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="I27" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="J27" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="K27" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="L27" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="M27" s="89"/>
-      <c r="N27" s="88"/>
-      <c r="O27" s="90"/>
-      <c r="P27" s="88"/>
-      <c r="Q27" s="88"/>
-      <c r="R27" s="91"/>
-      <c r="S27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="85">
-        <v>3</v>
-      </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="I28" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="J28" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="K28" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="L28" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="M28" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="N28" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="O28" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="P28" s="88"/>
-      <c r="Q28" s="88"/>
-      <c r="R28" s="91"/>
-      <c r="S28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="85">
-        <v>4</v>
-      </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="G29" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="N29" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="O29" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="P29" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q29" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="R29" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="85">
-        <v>5</v>
-      </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="G30" s="87" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="I30" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="J30" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="K30" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="L30" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="M30" s="34"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="87"/>
-      <c r="P30" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q30" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="R30" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="S30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="85">
-        <v>6</v>
-      </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="G31" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="H31" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="I31" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="J31" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="K31" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="L31" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="M31" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="N31" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="O31" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="P31" s="35"/>
-      <c r="Q31" s="35"/>
-      <c r="R31" s="33"/>
-      <c r="S31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="85">
-        <v>7</v>
-      </c>
-      <c r="C32" s="35"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="I32" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="J32" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="K32" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="L32" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="M32" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="N32" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="O32" s="87" t="s">
-        <v>11</v>
-      </c>
-      <c r="P32" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q32" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="R32" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="S32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="85">
-        <v>8</v>
-      </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="N33" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="O33" s="87" t="s">
-        <v>15</v>
-      </c>
-      <c r="P33" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q33" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="R33" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="S33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="86">
-        <v>9</v>
-      </c>
-      <c r="C34" s="93"/>
-      <c r="D34" s="94"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="93"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="93"/>
-      <c r="I34" s="93"/>
-      <c r="J34" s="93"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="94"/>
-      <c r="N34" s="93"/>
-      <c r="O34" s="95"/>
-      <c r="P34" s="93" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q34" s="93" t="s">
-        <v>15</v>
-      </c>
-      <c r="R34" s="96" t="s">
-        <v>11</v>
-      </c>
-      <c r="S34">
-        <v>0</v>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P24:R24"/>
+  <mergeCells count="9">
+    <mergeCell ref="T24:V24"/>
     <mergeCell ref="D24:G24"/>
-    <mergeCell ref="H24:L24"/>
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="N24:S24"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="C14:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Got it down to 2/8 tests failing for DP D
</commit_message>
<xml_diff>
--- a/Lab_2/Report/ControlSignals.xlsx
+++ b/Lab_2/Report/ControlSignals.xlsx
@@ -5,6 +5,7 @@
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="Data Path B" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="117">
   <si>
     <t>W_EN</t>
   </si>
@@ -369,6 +370,9 @@
   </si>
   <si>
     <t>Empty space should be treated as "don’t care" Ø</t>
+  </si>
+  <si>
+    <t>00</t>
   </si>
 </sst>
 </file>
@@ -408,6 +412,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="11">
@@ -975,7 +980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1043,6 +1048,56 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1062,15 +1117,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1100,79 +1146,26 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1754,6 +1747,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2068,6 +2062,7 @@
     <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S18" sqref="S18"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2146,7 +2141,7 @@
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="112" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="39" t="s">
@@ -2202,7 +2197,7 @@
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="69"/>
+      <c r="B4" s="113"/>
       <c r="C4" s="14" t="s">
         <v>53</v>
       </c>
@@ -2256,7 +2251,7 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="69"/>
+      <c r="B5" s="113"/>
       <c r="C5" s="12" t="s">
         <v>54</v>
       </c>
@@ -2310,7 +2305,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="70"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="14" t="s">
         <v>55</v>
       </c>
@@ -2364,7 +2359,7 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="115" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="40" t="s">
@@ -2420,7 +2415,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="69"/>
+      <c r="B8" s="113"/>
       <c r="C8" s="14" t="s">
         <v>53</v>
       </c>
@@ -2474,7 +2469,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="69"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="12" t="s">
         <v>54</v>
       </c>
@@ -2528,7 +2523,7 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="70"/>
+      <c r="B10" s="114"/>
       <c r="C10" s="14" t="s">
         <v>55</v>
       </c>
@@ -2582,7 +2577,7 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="115" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="40" t="s">
@@ -2638,7 +2633,7 @@
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="69"/>
+      <c r="B12" s="113"/>
       <c r="C12" s="14" t="s">
         <v>53</v>
       </c>
@@ -2692,7 +2687,7 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="12" t="s">
         <v>54</v>
       </c>
@@ -2746,7 +2741,7 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="70"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="14" t="s">
         <v>55</v>
       </c>
@@ -2800,7 +2795,7 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="115" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="40" t="s">
@@ -2856,7 +2851,7 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="69"/>
+      <c r="B16" s="113"/>
       <c r="C16" s="14" t="s">
         <v>53</v>
       </c>
@@ -2910,7 +2905,7 @@
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="69"/>
+      <c r="B17" s="113"/>
       <c r="C17" s="12" t="s">
         <v>54</v>
       </c>
@@ -2964,7 +2959,7 @@
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="70"/>
+      <c r="B18" s="114"/>
       <c r="C18" s="14" t="s">
         <v>67</v>
       </c>
@@ -3018,7 +3013,7 @@
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="113" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="40" t="s">
@@ -3074,7 +3069,7 @@
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="69"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="14" t="s">
         <v>67</v>
       </c>
@@ -3128,7 +3123,7 @@
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="69"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="12" t="s">
         <v>70</v>
       </c>
@@ -3182,7 +3177,7 @@
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="109" t="s">
         <v>69</v>
       </c>
       <c r="C22" s="45" t="s">
@@ -3238,7 +3233,7 @@
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="66"/>
+      <c r="B23" s="110"/>
       <c r="C23" s="49" t="s">
         <v>53</v>
       </c>
@@ -3292,7 +3287,7 @@
       </c>
     </row>
     <row r="24" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="67"/>
+      <c r="B24" s="111"/>
       <c r="C24" s="53" t="s">
         <v>54</v>
       </c>
@@ -3363,9 +3358,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3379,7 +3375,7 @@
     <col min="13" max="13" width="14" customWidth="1"/>
     <col min="14" max="15" width="10.7109375" customWidth="1"/>
     <col min="16" max="19" width="10.85546875" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3388,157 +3384,157 @@
       <c r="C2" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="119" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="81" t="s">
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="122" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="72" t="s">
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="124"/>
+      <c r="N2" s="125" t="s">
         <v>67</v>
       </c>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="75" t="s">
+      <c r="O2" s="126"/>
+      <c r="P2" s="126"/>
+      <c r="Q2" s="126"/>
+      <c r="R2" s="126"/>
+      <c r="S2" s="127"/>
+      <c r="T2" s="116" t="s">
         <v>91</v>
       </c>
-      <c r="U2" s="76"/>
-      <c r="V2" s="77"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="118"/>
     </row>
     <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="86" t="s">
+      <c r="C3" s="66"/>
+      <c r="D3" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="87" t="s">
+      <c r="F3" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="86" t="s">
+      <c r="H3" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="87" t="s">
+      <c r="I3" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="87" t="s">
+      <c r="J3" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="87" t="s">
+      <c r="K3" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="87" t="s">
+      <c r="L3" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="85" t="s">
+      <c r="M3" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="N3" s="87" t="s">
+      <c r="N3" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="87" t="s">
+      <c r="O3" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="P3" s="87" t="s">
+      <c r="P3" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="Q3" s="87" t="s">
+      <c r="Q3" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="87" t="s">
+      <c r="R3" s="68" t="s">
         <v>111</v>
       </c>
-      <c r="S3" s="87" t="s">
+      <c r="S3" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="T3" s="86" t="s">
+      <c r="T3" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="U3" s="87" t="s">
+      <c r="U3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="V3" s="88" t="s">
+      <c r="V3" s="69" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="114"/>
-      <c r="D4" s="115" t="s">
+      <c r="C4" s="89"/>
+      <c r="D4" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="116" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="116" t="s">
+      <c r="E4" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="114" t="s">
+      <c r="G4" s="89" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="115" t="s">
+      <c r="H4" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="116" t="s">
+      <c r="I4" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="J4" s="116" t="s">
+      <c r="J4" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="116" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="116" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="116" t="s">
+      <c r="K4" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="116" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="116" t="s">
+      <c r="N4" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="Q4" s="116" t="s">
-        <v>12</v>
-      </c>
-      <c r="R4" s="116" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="117">
+      <c r="Q4" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" s="91">
         <v>0</v>
       </c>
-      <c r="T4" s="115" t="s">
+      <c r="T4" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="116" t="s">
+      <c r="U4" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="118" t="s">
+      <c r="V4" s="92" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3546,62 +3542,62 @@
       <c r="B5" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="119"/>
-      <c r="D5" s="120" t="s">
+      <c r="C5" s="93"/>
+      <c r="D5" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="121" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="121" t="s">
+      <c r="E5" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="119" t="s">
+      <c r="G5" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="120" t="s">
+      <c r="H5" s="94" t="s">
         <v>104</v>
       </c>
-      <c r="I5" s="121" t="s">
+      <c r="I5" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="J5" s="121" t="s">
+      <c r="J5" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="121" t="s">
+      <c r="K5" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="121" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="121" t="s">
+      <c r="L5" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="120" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="P5" s="121" t="s">
+      <c r="N5" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="Q5" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="R5" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="S5" s="122">
+      <c r="Q5" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="R5" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="95">
         <v>0</v>
       </c>
-      <c r="T5" s="120" t="s">
+      <c r="T5" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="U5" s="121" t="s">
+      <c r="U5" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="V5" s="123" t="s">
+      <c r="V5" s="96" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3609,95 +3605,91 @@
       <c r="B6" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="125"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" s="125"/>
-      <c r="O6" s="126"/>
-      <c r="P6" s="126"/>
-      <c r="Q6" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="R6" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="S6" s="127">
+      <c r="C6" s="97"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="98"/>
+      <c r="O6" s="99"/>
+      <c r="P6" s="99"/>
+      <c r="Q6" s="99"/>
+      <c r="R6" s="99"/>
+      <c r="S6" s="99">
         <v>0</v>
       </c>
-      <c r="T6" s="125"/>
-      <c r="U6" s="126"/>
-      <c r="V6" s="128"/>
+      <c r="T6" s="98"/>
+      <c r="U6" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="V6" s="100"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="119"/>
-      <c r="D7" s="120" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="121" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="121" t="s">
+      <c r="C7" s="93"/>
+      <c r="D7" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="119" t="s">
+      <c r="G7" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="120" t="s">
-        <v>106</v>
-      </c>
-      <c r="I7" s="121" t="s">
+      <c r="H7" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="J7" s="121" t="s">
+      <c r="J7" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="121" t="s">
+      <c r="K7" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="M7" s="121" t="s">
+      <c r="M7" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="N7" s="120" t="s">
+      <c r="N7" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="O7" s="121" t="s">
+      <c r="O7" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="P7" s="121" t="s">
+      <c r="P7" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="Q7" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="R7" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="S7" s="122">
+      <c r="Q7" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="R7" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="S7" s="95">
         <v>0</v>
       </c>
-      <c r="T7" s="120" t="s">
-        <v>102</v>
-      </c>
-      <c r="U7" s="121" t="s">
-        <v>11</v>
-      </c>
-      <c r="V7" s="123" t="s">
+      <c r="T7" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="U7" s="95" t="s">
+        <v>15</v>
+      </c>
+      <c r="V7" s="96" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3705,62 +3697,62 @@
       <c r="B8" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="124"/>
-      <c r="D8" s="125" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="126" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="126" t="s">
+      <c r="C8" s="97"/>
+      <c r="D8" s="98" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="G8" s="124" t="s">
+      <c r="G8" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="125" t="s">
+      <c r="H8" s="98" t="s">
         <v>106</v>
       </c>
-      <c r="I8" s="126" t="s">
+      <c r="I8" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="J8" s="126" t="s">
+      <c r="J8" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="126" t="s">
+      <c r="K8" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="L8" s="126" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="126" t="s">
+      <c r="L8" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="N8" s="125" t="s">
+      <c r="N8" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="O8" s="126" t="s">
+      <c r="O8" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="P8" s="126" t="s">
+      <c r="P8" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="126" t="s">
+      <c r="Q8" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="R8" s="126" t="s">
+      <c r="R8" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="S8" s="127">
+      <c r="S8" s="99">
         <v>1</v>
       </c>
-      <c r="T8" s="125" t="s">
+      <c r="T8" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="U8" s="126" t="s">
+      <c r="U8" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="V8" s="128" t="s">
+      <c r="V8" s="100" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3768,100 +3760,100 @@
       <c r="B9" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="129"/>
-      <c r="D9" s="130" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="131" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="131" t="s">
+      <c r="C9" s="101"/>
+      <c r="D9" s="102" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="103" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="G9" s="129" t="s">
+      <c r="G9" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="H9" s="130" t="s">
+      <c r="H9" s="102" t="s">
         <v>103</v>
       </c>
-      <c r="I9" s="131" t="s">
+      <c r="I9" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="J9" s="131" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="131" t="s">
+      <c r="J9" s="103" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="103" t="s">
         <v>107</v>
       </c>
-      <c r="L9" s="131" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="131" t="s">
+      <c r="L9" s="103" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="N9" s="130" t="s">
+      <c r="N9" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="O9" s="131" t="s">
+      <c r="O9" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="131" t="s">
+      <c r="P9" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="Q9" s="131" t="s">
+      <c r="Q9" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="131" t="s">
-        <v>12</v>
-      </c>
-      <c r="S9" s="132">
+      <c r="R9" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="S9" s="103">
         <v>0</v>
       </c>
-      <c r="T9" s="130" t="s">
+      <c r="T9" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="U9" s="131" t="s">
+      <c r="U9" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="V9" s="133" t="s">
+      <c r="V9" s="104" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="107" t="s">
+      <c r="C14" s="128" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="107"/>
-      <c r="E14" s="107"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="107"/>
-      <c r="H14" s="107"/>
-      <c r="I14" s="107"/>
-      <c r="J14" s="107"/>
-      <c r="K14" s="107"/>
-      <c r="L14" s="108"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="128"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="128"/>
+      <c r="L14" s="129"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="90" t="s">
+      <c r="D15" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="91" t="s">
+      <c r="E15" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="92" t="s">
+      <c r="F15" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="105" t="s">
+      <c r="G15" s="82" t="s">
         <v>91</v>
       </c>
       <c r="H15" s="3"/>
@@ -3872,23 +3864,23 @@
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="102" t="s">
+      <c r="B16" s="79" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="93" t="s">
+      <c r="D16" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="94" t="s">
+      <c r="E16" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="95" t="s">
+      <c r="F16" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="96" t="s">
+      <c r="G16" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="97" t="s">
+      <c r="H16" s="78" t="s">
         <v>91</v>
       </c>
       <c r="I16" s="3"/>
@@ -3898,41 +3890,41 @@
       <c r="M16" s="3"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="102" t="s">
+      <c r="B17" s="79" t="s">
         <v>101</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="131"/>
+      <c r="G17" s="131"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="132"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="58"/>
       <c r="M17" s="3"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="102" t="s">
+      <c r="B18" s="79" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="93" t="s">
+      <c r="F18" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="98" t="s">
+      <c r="G18" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="H18" s="99" t="s">
+      <c r="H18" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="I18" s="100" t="s">
+      <c r="I18" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="101" t="s">
+      <c r="J18" s="78" t="s">
         <v>91</v>
       </c>
       <c r="K18" s="3"/>
@@ -3940,33 +3932,33 @@
       <c r="M18" s="3"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="102" t="s">
+      <c r="B19" s="79" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="93" t="s">
+      <c r="G19" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="98" t="s">
+      <c r="H19" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="99" t="s">
+      <c r="I19" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="J19" s="100" t="s">
+      <c r="J19" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="K19" s="101" t="s">
+      <c r="K19" s="78" t="s">
         <v>91</v>
       </c>
       <c r="L19" s="58"/>
       <c r="M19" s="3"/>
     </row>
     <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="103" t="s">
+      <c r="B20" s="80" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="59"/>
@@ -3974,19 +3966,19 @@
       <c r="E20" s="59"/>
       <c r="F20" s="59"/>
       <c r="G20" s="59"/>
-      <c r="H20" s="109" t="s">
+      <c r="H20" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="I20" s="110" t="s">
+      <c r="I20" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="J20" s="111" t="s">
+      <c r="J20" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="K20" s="112" t="s">
+      <c r="K20" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="L20" s="113" t="s">
+      <c r="L20" s="88" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3996,94 +3988,94 @@
       <c r="C24" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="78" t="s">
+      <c r="D24" s="119" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="81" t="s">
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="121"/>
+      <c r="H24" s="122" t="s">
         <v>89</v>
       </c>
-      <c r="I24" s="82"/>
-      <c r="J24" s="82"/>
-      <c r="K24" s="82"/>
-      <c r="L24" s="82"/>
-      <c r="M24" s="83"/>
-      <c r="N24" s="72" t="s">
+      <c r="I24" s="123"/>
+      <c r="J24" s="123"/>
+      <c r="K24" s="123"/>
+      <c r="L24" s="123"/>
+      <c r="M24" s="124"/>
+      <c r="N24" s="125" t="s">
         <v>67</v>
       </c>
-      <c r="O24" s="73"/>
-      <c r="P24" s="73"/>
-      <c r="Q24" s="73"/>
-      <c r="R24" s="73"/>
-      <c r="S24" s="74"/>
-      <c r="T24" s="75" t="s">
+      <c r="O24" s="126"/>
+      <c r="P24" s="126"/>
+      <c r="Q24" s="126"/>
+      <c r="R24" s="126"/>
+      <c r="S24" s="127"/>
+      <c r="T24" s="116" t="s">
         <v>91</v>
       </c>
-      <c r="U24" s="76"/>
-      <c r="V24" s="77"/>
+      <c r="U24" s="117"/>
+      <c r="V24" s="118"/>
     </row>
     <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="85"/>
-      <c r="D25" s="86" t="s">
+      <c r="C25" s="66"/>
+      <c r="D25" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="87" t="s">
+      <c r="E25" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="87" t="s">
+      <c r="F25" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="85" t="s">
+      <c r="G25" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="H25" s="86" t="s">
+      <c r="H25" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="I25" s="87" t="s">
+      <c r="I25" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="J25" s="87" t="s">
+      <c r="J25" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="K25" s="87" t="s">
+      <c r="K25" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="L25" s="87" t="s">
+      <c r="L25" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="M25" s="87" t="s">
+      <c r="M25" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="N25" s="87" t="s">
+      <c r="N25" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="O25" s="87" t="s">
+      <c r="O25" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="P25" s="87" t="s">
+      <c r="P25" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="Q25" s="87" t="s">
+      <c r="Q25" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="R25" s="87" t="s">
+      <c r="R25" s="68" t="s">
         <v>111</v>
       </c>
-      <c r="S25" s="87" t="s">
+      <c r="S25" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="T25" s="86" t="s">
+      <c r="T25" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="U25" s="87" t="s">
+      <c r="U25" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="V25" s="88" t="s">
+      <c r="V25" s="69" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4091,181 +4083,187 @@
       <c r="B26" s="62">
         <v>1</v>
       </c>
-      <c r="C26" s="134"/>
-      <c r="D26" s="115" t="s">
+      <c r="C26" s="105"/>
+      <c r="D26" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="116" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="116" t="s">
+      <c r="E26" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="114" t="s">
+      <c r="G26" s="89" t="s">
         <v>102</v>
       </c>
-      <c r="H26" s="135"/>
-      <c r="I26" s="135"/>
-      <c r="J26" s="135"/>
-      <c r="K26" s="135"/>
-      <c r="L26" s="135"/>
-      <c r="M26" s="135"/>
-      <c r="N26" s="136"/>
-      <c r="O26" s="117"/>
-      <c r="P26" s="117"/>
-      <c r="Q26" s="117"/>
-      <c r="R26" s="117"/>
-      <c r="S26" s="117">
+      <c r="H26" s="105"/>
+      <c r="I26" s="105"/>
+      <c r="J26" s="105"/>
+      <c r="K26" s="105"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="105"/>
+      <c r="N26" s="90"/>
+      <c r="O26" s="91"/>
+      <c r="P26" s="91"/>
+      <c r="Q26" s="91"/>
+      <c r="R26" s="91"/>
+      <c r="S26" s="91">
         <v>0</v>
       </c>
-      <c r="T26" s="137"/>
-      <c r="U26" s="135"/>
-      <c r="V26" s="138"/>
+      <c r="T26" s="133"/>
+      <c r="U26" s="105">
+        <v>0</v>
+      </c>
+      <c r="V26" s="134"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B27" s="60">
         <v>2</v>
       </c>
-      <c r="C27" s="126"/>
-      <c r="D27" s="120" t="s">
+      <c r="C27" s="99"/>
+      <c r="D27" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="121" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="121" t="s">
+      <c r="E27" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="119" t="s">
+      <c r="G27" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="H27" s="126" t="s">
+      <c r="H27" s="99" t="s">
         <v>104</v>
       </c>
-      <c r="I27" s="126" t="s">
+      <c r="I27" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="J27" s="126" t="s">
+      <c r="J27" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="K27" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="L27" s="126" t="s">
-        <v>22</v>
-      </c>
-      <c r="M27" s="126" t="s">
+      <c r="K27" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="N27" s="139"/>
-      <c r="O27" s="122"/>
-      <c r="P27" s="122"/>
-      <c r="Q27" s="122"/>
-      <c r="R27" s="122"/>
-      <c r="S27" s="122">
+      <c r="N27" s="94"/>
+      <c r="O27" s="95"/>
+      <c r="P27" s="95"/>
+      <c r="Q27" s="95"/>
+      <c r="R27" s="95"/>
+      <c r="S27" s="95">
         <v>0</v>
       </c>
-      <c r="T27" s="140"/>
-      <c r="U27" s="127"/>
-      <c r="V27" s="141"/>
+      <c r="T27" s="98"/>
+      <c r="U27" s="99">
+        <v>0</v>
+      </c>
+      <c r="V27" s="100"/>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B28" s="60">
         <v>3</v>
       </c>
-      <c r="C28" s="121"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="126"/>
-      <c r="F28" s="126"/>
-      <c r="G28" s="124"/>
-      <c r="H28" s="121" t="s">
+      <c r="C28" s="95"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="95" t="s">
         <v>104</v>
       </c>
-      <c r="I28" s="121" t="s">
+      <c r="I28" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="J28" s="121" t="s">
+      <c r="J28" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="K28" s="121" t="s">
+      <c r="K28" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="L28" s="121" t="s">
-        <v>22</v>
-      </c>
-      <c r="M28" s="121" t="s">
-        <v>43</v>
-      </c>
-      <c r="N28" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="O28" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="P28" s="126" t="s">
+      <c r="L28" s="95" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="95" t="s">
+        <v>19</v>
+      </c>
+      <c r="N28" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="O28" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="P28" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="Q28" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="R28" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="S28" s="127">
+      <c r="Q28" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="R28" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="S28" s="99">
         <v>0</v>
       </c>
-      <c r="T28" s="139"/>
-      <c r="U28" s="122"/>
-      <c r="V28" s="142"/>
+      <c r="T28" s="94"/>
+      <c r="U28" s="95">
+        <v>0</v>
+      </c>
+      <c r="V28" s="96"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B29" s="60">
         <v>4</v>
       </c>
-      <c r="C29" s="126"/>
-      <c r="D29" s="120" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="121" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="121" t="s">
+      <c r="C29" s="99"/>
+      <c r="D29" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="G29" s="119" t="s">
+      <c r="G29" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="H29" s="126"/>
-      <c r="I29" s="126"/>
-      <c r="J29" s="126"/>
-      <c r="K29" s="126"/>
-      <c r="L29" s="126"/>
-      <c r="M29" s="126"/>
-      <c r="N29" s="120" t="s">
-        <v>12</v>
-      </c>
-      <c r="O29" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="P29" s="121" t="s">
+      <c r="H29" s="99"/>
+      <c r="I29" s="99"/>
+      <c r="J29" s="99"/>
+      <c r="K29" s="99"/>
+      <c r="L29" s="99"/>
+      <c r="M29" s="99"/>
+      <c r="N29" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="P29" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="Q29" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="R29" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="S29" s="122">
+      <c r="Q29" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="R29" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="S29" s="95">
         <v>0</v>
       </c>
-      <c r="T29" s="125" t="s">
+      <c r="T29" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="U29" s="126" t="s">
+      <c r="U29" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="V29" s="128" t="s">
+      <c r="V29" s="100" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4273,52 +4271,52 @@
       <c r="B30" s="60">
         <v>5</v>
       </c>
-      <c r="C30" s="121"/>
-      <c r="D30" s="125" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="126" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="126" t="s">
+      <c r="C30" s="95"/>
+      <c r="D30" s="98" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="G30" s="124" t="s">
+      <c r="G30" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="121" t="s">
-        <v>106</v>
-      </c>
-      <c r="I30" s="121" t="s">
+      <c r="H30" s="95" t="s">
+        <v>116</v>
+      </c>
+      <c r="I30" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="J30" s="121" t="s">
+      <c r="J30" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="K30" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="L30" s="121" t="s">
+      <c r="K30" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="M30" s="121" t="s">
-        <v>43</v>
-      </c>
-      <c r="N30" s="125"/>
-      <c r="O30" s="126"/>
-      <c r="P30" s="126"/>
-      <c r="Q30" s="126"/>
-      <c r="R30" s="126"/>
-      <c r="S30" s="127">
+      <c r="M30" s="95" t="s">
+        <v>19</v>
+      </c>
+      <c r="N30" s="98"/>
+      <c r="O30" s="99"/>
+      <c r="P30" s="99"/>
+      <c r="Q30" s="99"/>
+      <c r="R30" s="99"/>
+      <c r="S30" s="99">
         <v>0</v>
       </c>
-      <c r="T30" s="120" t="s">
+      <c r="T30" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="U30" s="121" t="s">
+      <c r="U30" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="V30" s="123" t="s">
+      <c r="V30" s="96" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4326,111 +4324,113 @@
       <c r="B31" s="60">
         <v>6</v>
       </c>
-      <c r="C31" s="126"/>
-      <c r="D31" s="120" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="121" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="121" t="s">
+      <c r="C31" s="99"/>
+      <c r="D31" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="G31" s="119" t="s">
+      <c r="G31" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="H31" s="126" t="s">
+      <c r="H31" s="99" t="s">
         <v>106</v>
       </c>
-      <c r="I31" s="126" t="s">
+      <c r="I31" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="J31" s="126" t="s">
+      <c r="J31" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="K31" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="L31" s="126" t="s">
-        <v>22</v>
-      </c>
-      <c r="M31" s="126" t="s">
-        <v>43</v>
-      </c>
-      <c r="N31" s="120" t="s">
-        <v>12</v>
-      </c>
-      <c r="O31" s="121" t="s">
+      <c r="K31" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="M31" s="99" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="O31" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="P31" s="121" t="s">
+      <c r="P31" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="Q31" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="R31" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="S31" s="122">
+      <c r="Q31" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="R31" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="S31" s="95">
         <v>0</v>
       </c>
-      <c r="T31" s="125"/>
-      <c r="U31" s="126"/>
-      <c r="V31" s="128"/>
+      <c r="T31" s="98"/>
+      <c r="U31" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="V31" s="100"/>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B32" s="60">
         <v>7</v>
       </c>
-      <c r="C32" s="121"/>
-      <c r="D32" s="125"/>
-      <c r="E32" s="126"/>
-      <c r="F32" s="126"/>
-      <c r="G32" s="124"/>
-      <c r="H32" s="121" t="s">
+      <c r="C32" s="95"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="99"/>
+      <c r="F32" s="99"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="I32" s="121" t="s">
+      <c r="I32" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="J32" s="121" t="s">
-        <v>22</v>
-      </c>
-      <c r="K32" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="L32" s="121" t="s">
-        <v>22</v>
-      </c>
-      <c r="M32" s="121" t="s">
+      <c r="J32" s="95" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="95" t="s">
+        <v>22</v>
+      </c>
+      <c r="M32" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="N32" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="O32" s="126" t="s">
+      <c r="N32" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="P32" s="126" t="s">
+      <c r="P32" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="Q32" s="126" t="s">
+      <c r="Q32" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="R32" s="126" t="s">
+      <c r="R32" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="S32" s="127">
+      <c r="S32" s="99">
         <v>1</v>
       </c>
-      <c r="T32" s="120" t="s">
-        <v>102</v>
-      </c>
-      <c r="U32" s="121" t="s">
-        <v>11</v>
-      </c>
-      <c r="V32" s="123" t="s">
+      <c r="T32" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="U32" s="95" t="s">
+        <v>15</v>
+      </c>
+      <c r="V32" s="96" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4438,42 +4438,42 @@
       <c r="B33" s="60">
         <v>8</v>
       </c>
-      <c r="C33" s="126"/>
-      <c r="D33" s="120"/>
-      <c r="E33" s="121"/>
-      <c r="F33" s="121"/>
-      <c r="G33" s="119"/>
-      <c r="H33" s="126"/>
-      <c r="I33" s="126"/>
-      <c r="J33" s="126"/>
-      <c r="K33" s="126"/>
-      <c r="L33" s="126"/>
-      <c r="M33" s="126"/>
-      <c r="N33" s="120" t="s">
+      <c r="C33" s="99"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="95"/>
+      <c r="G33" s="93"/>
+      <c r="H33" s="99"/>
+      <c r="I33" s="99"/>
+      <c r="J33" s="99"/>
+      <c r="K33" s="99"/>
+      <c r="L33" s="99"/>
+      <c r="M33" s="99"/>
+      <c r="N33" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="O33" s="121" t="s">
+      <c r="O33" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="P33" s="121" t="s">
+      <c r="P33" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="Q33" s="121" t="s">
+      <c r="Q33" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="R33" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="S33" s="122">
+      <c r="R33" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="S33" s="95">
         <v>0</v>
       </c>
-      <c r="T33" s="125" t="s">
+      <c r="T33" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="U33" s="126" t="s">
+      <c r="U33" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="V33" s="128" t="s">
+      <c r="V33" s="100" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4481,32 +4481,32 @@
       <c r="B34" s="61">
         <v>9</v>
       </c>
-      <c r="C34" s="131"/>
-      <c r="D34" s="143"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="145"/>
-      <c r="H34" s="131"/>
-      <c r="I34" s="131"/>
-      <c r="J34" s="131"/>
-      <c r="K34" s="131"/>
-      <c r="L34" s="131"/>
-      <c r="M34" s="131"/>
-      <c r="N34" s="143"/>
-      <c r="O34" s="144"/>
-      <c r="P34" s="144"/>
-      <c r="Q34" s="144"/>
-      <c r="R34" s="144"/>
-      <c r="S34" s="146">
+      <c r="C34" s="103"/>
+      <c r="D34" s="106"/>
+      <c r="E34" s="107"/>
+      <c r="F34" s="107"/>
+      <c r="G34" s="108"/>
+      <c r="H34" s="103"/>
+      <c r="I34" s="103"/>
+      <c r="J34" s="103"/>
+      <c r="K34" s="103"/>
+      <c r="L34" s="103"/>
+      <c r="M34" s="103"/>
+      <c r="N34" s="106"/>
+      <c r="O34" s="107"/>
+      <c r="P34" s="107"/>
+      <c r="Q34" s="107"/>
+      <c r="R34" s="107"/>
+      <c r="S34" s="107">
         <v>0</v>
       </c>
-      <c r="T34" s="130" t="s">
+      <c r="T34" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="U34" s="131" t="s">
+      <c r="U34" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="V34" s="133" t="s">
+      <c r="V34" s="104" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Down to one error
</commit_message>
<xml_diff>
--- a/Lab_2/Report/ControlSignals.xlsx
+++ b/Lab_2/Report/ControlSignals.xlsx
@@ -5,7 +5,6 @@
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="Data Path B" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="116">
   <si>
     <t>W_EN</t>
   </si>
@@ -370,9 +369,6 @@
   </si>
   <si>
     <t>Empty space should be treated as "don’t care" Ø</t>
-  </si>
-  <si>
-    <t>00</t>
   </si>
 </sst>
 </file>
@@ -1098,6 +1094,11 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1161,11 +1162,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1747,7 +1743,6 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2062,7 +2057,6 @@
     <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S18" sqref="S18"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2141,7 +2135,7 @@
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="117" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="39" t="s">
@@ -2197,7 +2191,7 @@
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="113"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="14" t="s">
         <v>53</v>
       </c>
@@ -2251,7 +2245,7 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="113"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="12" t="s">
         <v>54</v>
       </c>
@@ -2305,7 +2299,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="114"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="14" t="s">
         <v>55</v>
       </c>
@@ -2359,7 +2353,7 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="120" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="40" t="s">
@@ -2415,7 +2409,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="113"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="14" t="s">
         <v>53</v>
       </c>
@@ -2469,7 +2463,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="113"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="12" t="s">
         <v>54</v>
       </c>
@@ -2523,7 +2517,7 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="114"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="14" t="s">
         <v>55</v>
       </c>
@@ -2577,7 +2571,7 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="120" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="40" t="s">
@@ -2633,7 +2627,7 @@
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="113"/>
+      <c r="B12" s="118"/>
       <c r="C12" s="14" t="s">
         <v>53</v>
       </c>
@@ -2687,7 +2681,7 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="113"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="12" t="s">
         <v>54</v>
       </c>
@@ -2741,7 +2735,7 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="114"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="14" t="s">
         <v>55</v>
       </c>
@@ -2795,7 +2789,7 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="115" t="s">
+      <c r="B15" s="120" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="40" t="s">
@@ -2851,7 +2845,7 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="113"/>
+      <c r="B16" s="118"/>
       <c r="C16" s="14" t="s">
         <v>53</v>
       </c>
@@ -2905,7 +2899,7 @@
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="113"/>
+      <c r="B17" s="118"/>
       <c r="C17" s="12" t="s">
         <v>54</v>
       </c>
@@ -2959,7 +2953,7 @@
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="114"/>
+      <c r="B18" s="119"/>
       <c r="C18" s="14" t="s">
         <v>67</v>
       </c>
@@ -3013,7 +3007,7 @@
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="113" t="s">
+      <c r="B19" s="118" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="40" t="s">
@@ -3069,7 +3063,7 @@
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="113"/>
+      <c r="B20" s="118"/>
       <c r="C20" s="14" t="s">
         <v>67</v>
       </c>
@@ -3123,7 +3117,7 @@
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="113"/>
+      <c r="B21" s="118"/>
       <c r="C21" s="12" t="s">
         <v>70</v>
       </c>
@@ -3177,7 +3171,7 @@
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="109" t="s">
+      <c r="B22" s="114" t="s">
         <v>69</v>
       </c>
       <c r="C22" s="45" t="s">
@@ -3233,7 +3227,7 @@
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="110"/>
+      <c r="B23" s="115"/>
       <c r="C23" s="49" t="s">
         <v>53</v>
       </c>
@@ -3287,7 +3281,7 @@
       </c>
     </row>
     <row r="24" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="111"/>
+      <c r="B24" s="116"/>
       <c r="C24" s="53" t="s">
         <v>54</v>
       </c>
@@ -3359,9 +3353,8 @@
   <dimension ref="B1:V37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3384,33 +3377,33 @@
       <c r="C2" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="119" t="s">
+      <c r="D2" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="122" t="s">
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="127" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="123"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="125" t="s">
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="129"/>
+      <c r="N2" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="O2" s="126"/>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="126"/>
-      <c r="R2" s="126"/>
-      <c r="S2" s="127"/>
-      <c r="T2" s="116" t="s">
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+      <c r="S2" s="132"/>
+      <c r="T2" s="121" t="s">
         <v>91</v>
       </c>
-      <c r="U2" s="117"/>
-      <c r="V2" s="118"/>
+      <c r="U2" s="122"/>
+      <c r="V2" s="123"/>
     </row>
     <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="65" t="s">
@@ -3642,13 +3635,13 @@
         <v>10</v>
       </c>
       <c r="F7" s="95" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="G7" s="93" t="s">
         <v>102</v>
       </c>
       <c r="H7" s="94" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="I7" s="95" t="s">
         <v>103</v>
@@ -3824,18 +3817,18 @@
       <c r="B14" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="128" t="s">
+      <c r="C14" s="133" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="128"/>
-      <c r="E14" s="128"/>
-      <c r="F14" s="128"/>
-      <c r="G14" s="128"/>
-      <c r="H14" s="128"/>
-      <c r="I14" s="128"/>
-      <c r="J14" s="128"/>
-      <c r="K14" s="128"/>
-      <c r="L14" s="129"/>
+      <c r="D14" s="133"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="133"/>
+      <c r="I14" s="133"/>
+      <c r="J14" s="133"/>
+      <c r="K14" s="133"/>
+      <c r="L14" s="134"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="79" t="s">
@@ -3895,11 +3888,11 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
-      <c r="G17" s="131"/>
-      <c r="H17" s="131"/>
-      <c r="I17" s="132"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="110"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="111"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="58"/>
@@ -3988,33 +3981,33 @@
       <c r="C24" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="119" t="s">
+      <c r="D24" s="124" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="120"/>
-      <c r="F24" s="120"/>
-      <c r="G24" s="121"/>
-      <c r="H24" s="122" t="s">
+      <c r="E24" s="125"/>
+      <c r="F24" s="125"/>
+      <c r="G24" s="126"/>
+      <c r="H24" s="127" t="s">
         <v>89</v>
       </c>
-      <c r="I24" s="123"/>
-      <c r="J24" s="123"/>
-      <c r="K24" s="123"/>
-      <c r="L24" s="123"/>
-      <c r="M24" s="124"/>
-      <c r="N24" s="125" t="s">
+      <c r="I24" s="128"/>
+      <c r="J24" s="128"/>
+      <c r="K24" s="128"/>
+      <c r="L24" s="128"/>
+      <c r="M24" s="129"/>
+      <c r="N24" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="O24" s="126"/>
-      <c r="P24" s="126"/>
-      <c r="Q24" s="126"/>
-      <c r="R24" s="126"/>
-      <c r="S24" s="127"/>
-      <c r="T24" s="116" t="s">
+      <c r="O24" s="131"/>
+      <c r="P24" s="131"/>
+      <c r="Q24" s="131"/>
+      <c r="R24" s="131"/>
+      <c r="S24" s="132"/>
+      <c r="T24" s="121" t="s">
         <v>91</v>
       </c>
-      <c r="U24" s="117"/>
-      <c r="V24" s="118"/>
+      <c r="U24" s="122"/>
+      <c r="V24" s="123"/>
     </row>
     <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="65" t="s">
@@ -4110,11 +4103,11 @@
       <c r="S26" s="91">
         <v>0</v>
       </c>
-      <c r="T26" s="133"/>
+      <c r="T26" s="112"/>
       <c r="U26" s="105">
         <v>0</v>
       </c>
-      <c r="V26" s="134"/>
+      <c r="V26" s="113"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B27" s="60">
@@ -4228,7 +4221,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="95" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="G29" s="93" t="s">
         <v>102</v>
@@ -4285,7 +4278,7 @@
         <v>15</v>
       </c>
       <c r="H30" s="95" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="I30" s="95" t="s">
         <v>103</v>

</xml_diff>